<commit_message>
DATABASE에 대한 modbus 실행 확인
</commit_message>
<xml_diff>
--- a/uploads/Modbus.xlsx
+++ b/uploads/Modbus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghks2\Bems\prac\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A59B8E-2375-4509-B223-829BDDE8792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF775E3-79AB-456B-9CF0-191577883693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2362,7 +2362,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1:T1048576"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
@@ -2388,1456 +2388,1456 @@
     <col min="19" max="19" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.83203125" style="4" customWidth="1"/>
     <col min="21" max="21" width="15.58203125" style="4" customWidth="1"/>
-    <col min="22" max="255" width="9" style="4"/>
-    <col min="256" max="256" width="37.83203125" style="4" customWidth="1"/>
-    <col min="257" max="257" width="6.58203125" style="4" customWidth="1"/>
-    <col min="258" max="258" width="9" style="4"/>
-    <col min="259" max="259" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="12.75" style="4" customWidth="1"/>
-    <col min="267" max="267" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="14.08203125" style="4" customWidth="1"/>
-    <col min="269" max="269" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="12.83203125" style="4" customWidth="1"/>
-    <col min="277" max="277" width="15.58203125" style="4" customWidth="1"/>
-    <col min="278" max="511" width="9" style="4"/>
-    <col min="512" max="512" width="37.83203125" style="4" customWidth="1"/>
-    <col min="513" max="513" width="6.58203125" style="4" customWidth="1"/>
-    <col min="514" max="514" width="9" style="4"/>
-    <col min="515" max="515" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="517" max="517" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="518" max="518" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="519" max="519" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="521" max="521" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="522" max="522" width="12.75" style="4" customWidth="1"/>
-    <col min="523" max="523" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="524" max="524" width="14.08203125" style="4" customWidth="1"/>
-    <col min="525" max="525" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="526" max="526" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="528" max="528" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="529" max="529" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="530" max="530" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="531" max="531" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="532" max="532" width="12.83203125" style="4" customWidth="1"/>
-    <col min="533" max="533" width="15.58203125" style="4" customWidth="1"/>
-    <col min="534" max="767" width="9" style="4"/>
-    <col min="768" max="768" width="37.83203125" style="4" customWidth="1"/>
-    <col min="769" max="769" width="6.58203125" style="4" customWidth="1"/>
-    <col min="770" max="770" width="9" style="4"/>
-    <col min="771" max="771" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="772" max="772" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="773" max="773" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="774" max="774" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="775" max="775" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="777" max="777" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="778" max="778" width="12.75" style="4" customWidth="1"/>
-    <col min="779" max="779" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="780" max="780" width="14.08203125" style="4" customWidth="1"/>
-    <col min="781" max="781" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="782" max="782" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="783" max="783" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="784" max="784" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="785" max="785" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="786" max="786" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="787" max="787" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="788" max="788" width="12.83203125" style="4" customWidth="1"/>
-    <col min="789" max="789" width="15.58203125" style="4" customWidth="1"/>
-    <col min="790" max="1023" width="9" style="4"/>
-    <col min="1024" max="1024" width="37.83203125" style="4" customWidth="1"/>
-    <col min="1025" max="1025" width="6.58203125" style="4" customWidth="1"/>
-    <col min="1026" max="1026" width="9" style="4"/>
-    <col min="1027" max="1027" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1028" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1029" max="1029" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1030" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="1031" max="1031" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1033" max="1033" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1034" width="12.75" style="4" customWidth="1"/>
-    <col min="1035" max="1035" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1036" max="1036" width="14.08203125" style="4" customWidth="1"/>
-    <col min="1037" max="1037" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1038" max="1038" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="1039" max="1039" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="1040" max="1040" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1041" max="1041" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1042" max="1042" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1043" max="1043" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1044" max="1044" width="12.83203125" style="4" customWidth="1"/>
-    <col min="1045" max="1045" width="15.58203125" style="4" customWidth="1"/>
-    <col min="1046" max="1279" width="9" style="4"/>
-    <col min="1280" max="1280" width="37.83203125" style="4" customWidth="1"/>
-    <col min="1281" max="1281" width="6.58203125" style="4" customWidth="1"/>
-    <col min="1282" max="1282" width="9" style="4"/>
-    <col min="1283" max="1283" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1284" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1285" max="1285" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1286" max="1286" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="1287" max="1287" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1289" max="1289" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="1290" max="1290" width="12.75" style="4" customWidth="1"/>
-    <col min="1291" max="1291" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1292" max="1292" width="14.08203125" style="4" customWidth="1"/>
-    <col min="1293" max="1293" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1294" max="1294" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="1295" max="1295" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="1296" max="1296" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1297" max="1297" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1298" max="1298" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1299" max="1299" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1300" max="1300" width="12.83203125" style="4" customWidth="1"/>
-    <col min="1301" max="1301" width="15.58203125" style="4" customWidth="1"/>
-    <col min="1302" max="1535" width="9" style="4"/>
-    <col min="1536" max="1536" width="37.83203125" style="4" customWidth="1"/>
-    <col min="1537" max="1537" width="6.58203125" style="4" customWidth="1"/>
-    <col min="1538" max="1538" width="9" style="4"/>
-    <col min="1539" max="1539" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1540" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1541" max="1541" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1542" max="1542" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="1543" max="1543" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1545" max="1545" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="1546" max="1546" width="12.75" style="4" customWidth="1"/>
-    <col min="1547" max="1547" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1548" max="1548" width="14.08203125" style="4" customWidth="1"/>
-    <col min="1549" max="1549" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1550" max="1550" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="1551" max="1551" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="1552" max="1552" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1553" max="1553" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1554" max="1554" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1555" max="1555" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1556" max="1556" width="12.83203125" style="4" customWidth="1"/>
-    <col min="1557" max="1557" width="15.58203125" style="4" customWidth="1"/>
-    <col min="1558" max="1791" width="9" style="4"/>
-    <col min="1792" max="1792" width="37.83203125" style="4" customWidth="1"/>
-    <col min="1793" max="1793" width="6.58203125" style="4" customWidth="1"/>
-    <col min="1794" max="1794" width="9" style="4"/>
-    <col min="1795" max="1795" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1796" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1797" max="1797" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1798" max="1798" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="1799" max="1799" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1801" max="1801" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="1802" max="1802" width="12.75" style="4" customWidth="1"/>
-    <col min="1803" max="1803" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="1804" max="1804" width="14.08203125" style="4" customWidth="1"/>
-    <col min="1805" max="1805" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1806" max="1806" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="1807" max="1807" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="1808" max="1808" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1809" max="1809" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1810" max="1810" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1811" max="1811" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="1812" max="1812" width="12.83203125" style="4" customWidth="1"/>
-    <col min="1813" max="1813" width="15.58203125" style="4" customWidth="1"/>
-    <col min="1814" max="2047" width="9" style="4"/>
-    <col min="2048" max="2048" width="37.83203125" style="4" customWidth="1"/>
-    <col min="2049" max="2049" width="6.58203125" style="4" customWidth="1"/>
-    <col min="2050" max="2050" width="9" style="4"/>
-    <col min="2051" max="2051" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2052" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2053" max="2053" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2054" max="2054" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2055" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2057" max="2057" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2058" max="2058" width="12.75" style="4" customWidth="1"/>
-    <col min="2059" max="2059" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2060" max="2060" width="14.08203125" style="4" customWidth="1"/>
-    <col min="2061" max="2061" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2062" max="2062" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2063" max="2063" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2064" max="2064" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2065" max="2065" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2066" max="2066" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2067" max="2067" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2068" max="2068" width="12.83203125" style="4" customWidth="1"/>
-    <col min="2069" max="2069" width="15.58203125" style="4" customWidth="1"/>
-    <col min="2070" max="2303" width="9" style="4"/>
-    <col min="2304" max="2304" width="37.83203125" style="4" customWidth="1"/>
-    <col min="2305" max="2305" width="6.58203125" style="4" customWidth="1"/>
-    <col min="2306" max="2306" width="9" style="4"/>
-    <col min="2307" max="2307" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2308" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2309" max="2309" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2310" max="2310" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="2311" max="2311" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2313" max="2313" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2314" max="2314" width="12.75" style="4" customWidth="1"/>
-    <col min="2315" max="2315" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2316" max="2316" width="14.08203125" style="4" customWidth="1"/>
-    <col min="2317" max="2317" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2318" max="2318" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2319" max="2319" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2320" max="2320" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2321" max="2321" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2322" max="2322" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2323" max="2323" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2324" max="2324" width="12.83203125" style="4" customWidth="1"/>
-    <col min="2325" max="2325" width="15.58203125" style="4" customWidth="1"/>
-    <col min="2326" max="2559" width="9" style="4"/>
-    <col min="2560" max="2560" width="37.83203125" style="4" customWidth="1"/>
-    <col min="2561" max="2561" width="6.58203125" style="4" customWidth="1"/>
-    <col min="2562" max="2562" width="9" style="4"/>
-    <col min="2563" max="2563" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2564" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2565" max="2565" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2566" max="2566" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="2567" max="2567" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2569" max="2569" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2570" max="2570" width="12.75" style="4" customWidth="1"/>
-    <col min="2571" max="2571" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2572" max="2572" width="14.08203125" style="4" customWidth="1"/>
-    <col min="2573" max="2573" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2574" max="2574" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2575" max="2575" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2576" max="2576" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2577" max="2577" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2578" max="2578" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2579" max="2579" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2580" max="2580" width="12.83203125" style="4" customWidth="1"/>
-    <col min="2581" max="2581" width="15.58203125" style="4" customWidth="1"/>
-    <col min="2582" max="2815" width="9" style="4"/>
-    <col min="2816" max="2816" width="37.83203125" style="4" customWidth="1"/>
-    <col min="2817" max="2817" width="6.58203125" style="4" customWidth="1"/>
-    <col min="2818" max="2818" width="9" style="4"/>
-    <col min="2819" max="2819" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2820" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2821" max="2821" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2822" max="2822" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="2823" max="2823" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2825" max="2825" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2826" max="2826" width="12.75" style="4" customWidth="1"/>
-    <col min="2827" max="2827" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2828" max="2828" width="14.08203125" style="4" customWidth="1"/>
-    <col min="2829" max="2829" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2830" max="2830" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2831" max="2831" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2832" max="2832" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2833" max="2833" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2834" max="2834" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2835" max="2835" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2836" max="2836" width="12.83203125" style="4" customWidth="1"/>
-    <col min="2837" max="2837" width="15.58203125" style="4" customWidth="1"/>
-    <col min="2838" max="3071" width="9" style="4"/>
-    <col min="3072" max="3072" width="37.83203125" style="4" customWidth="1"/>
-    <col min="3073" max="3073" width="6.58203125" style="4" customWidth="1"/>
-    <col min="3074" max="3074" width="9" style="4"/>
-    <col min="3075" max="3075" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3076" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3077" max="3077" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3078" max="3078" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3079" max="3079" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3081" max="3081" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3082" max="3082" width="12.75" style="4" customWidth="1"/>
-    <col min="3083" max="3083" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3084" max="3084" width="14.08203125" style="4" customWidth="1"/>
-    <col min="3085" max="3085" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3086" max="3086" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3087" max="3087" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3088" max="3088" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3089" max="3089" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3090" max="3090" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3091" max="3091" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3092" max="3092" width="12.83203125" style="4" customWidth="1"/>
-    <col min="3093" max="3093" width="15.58203125" style="4" customWidth="1"/>
-    <col min="3094" max="3327" width="9" style="4"/>
-    <col min="3328" max="3328" width="37.83203125" style="4" customWidth="1"/>
-    <col min="3329" max="3329" width="6.58203125" style="4" customWidth="1"/>
-    <col min="3330" max="3330" width="9" style="4"/>
-    <col min="3331" max="3331" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3332" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3333" max="3333" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3334" max="3334" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3335" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3337" max="3337" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3338" max="3338" width="12.75" style="4" customWidth="1"/>
-    <col min="3339" max="3339" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3340" max="3340" width="14.08203125" style="4" customWidth="1"/>
-    <col min="3341" max="3341" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3342" max="3342" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3343" max="3343" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3344" max="3344" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3345" max="3345" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3346" max="3346" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3347" max="3347" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3348" max="3348" width="12.83203125" style="4" customWidth="1"/>
-    <col min="3349" max="3349" width="15.58203125" style="4" customWidth="1"/>
-    <col min="3350" max="3583" width="9" style="4"/>
-    <col min="3584" max="3584" width="37.83203125" style="4" customWidth="1"/>
-    <col min="3585" max="3585" width="6.58203125" style="4" customWidth="1"/>
-    <col min="3586" max="3586" width="9" style="4"/>
-    <col min="3587" max="3587" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3588" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3589" max="3589" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3590" max="3590" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3591" max="3591" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3593" max="3593" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3594" max="3594" width="12.75" style="4" customWidth="1"/>
-    <col min="3595" max="3595" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3596" max="3596" width="14.08203125" style="4" customWidth="1"/>
-    <col min="3597" max="3597" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3598" max="3598" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3599" max="3599" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3600" max="3600" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3601" max="3601" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3602" max="3602" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3603" max="3603" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3604" max="3604" width="12.83203125" style="4" customWidth="1"/>
-    <col min="3605" max="3605" width="15.58203125" style="4" customWidth="1"/>
-    <col min="3606" max="3839" width="9" style="4"/>
-    <col min="3840" max="3840" width="37.83203125" style="4" customWidth="1"/>
-    <col min="3841" max="3841" width="6.58203125" style="4" customWidth="1"/>
-    <col min="3842" max="3842" width="9" style="4"/>
-    <col min="3843" max="3843" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3844" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3845" max="3845" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3846" max="3846" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="3847" max="3847" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3849" max="3849" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3850" max="3850" width="12.75" style="4" customWidth="1"/>
-    <col min="3851" max="3851" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3852" max="3852" width="14.08203125" style="4" customWidth="1"/>
-    <col min="3853" max="3853" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3854" max="3854" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3855" max="3855" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3856" max="3856" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3857" max="3857" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3858" max="3858" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3859" max="3859" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3860" max="3860" width="12.83203125" style="4" customWidth="1"/>
-    <col min="3861" max="3861" width="15.58203125" style="4" customWidth="1"/>
-    <col min="3862" max="4095" width="9" style="4"/>
-    <col min="4096" max="4096" width="37.83203125" style="4" customWidth="1"/>
-    <col min="4097" max="4097" width="6.58203125" style="4" customWidth="1"/>
-    <col min="4098" max="4098" width="9" style="4"/>
-    <col min="4099" max="4099" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4100" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4101" max="4101" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4102" max="4102" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4103" max="4103" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4105" max="4105" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="4106" max="4106" width="12.75" style="4" customWidth="1"/>
-    <col min="4107" max="4107" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4108" max="4108" width="14.08203125" style="4" customWidth="1"/>
-    <col min="4109" max="4109" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4110" max="4110" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4111" max="4111" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4112" max="4112" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4113" max="4113" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4114" max="4114" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4115" max="4115" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4116" max="4116" width="12.83203125" style="4" customWidth="1"/>
-    <col min="4117" max="4117" width="15.58203125" style="4" customWidth="1"/>
-    <col min="4118" max="4351" width="9" style="4"/>
-    <col min="4352" max="4352" width="37.83203125" style="4" customWidth="1"/>
-    <col min="4353" max="4353" width="6.58203125" style="4" customWidth="1"/>
-    <col min="4354" max="4354" width="9" style="4"/>
-    <col min="4355" max="4355" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4356" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4357" max="4357" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4358" max="4358" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4359" max="4359" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4361" max="4361" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="4362" max="4362" width="12.75" style="4" customWidth="1"/>
-    <col min="4363" max="4363" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4364" max="4364" width="14.08203125" style="4" customWidth="1"/>
-    <col min="4365" max="4365" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4366" max="4366" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4367" max="4367" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4368" max="4368" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4369" max="4369" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4370" max="4370" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4371" max="4371" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4372" max="4372" width="12.83203125" style="4" customWidth="1"/>
-    <col min="4373" max="4373" width="15.58203125" style="4" customWidth="1"/>
-    <col min="4374" max="4607" width="9" style="4"/>
-    <col min="4608" max="4608" width="37.83203125" style="4" customWidth="1"/>
-    <col min="4609" max="4609" width="6.58203125" style="4" customWidth="1"/>
-    <col min="4610" max="4610" width="9" style="4"/>
-    <col min="4611" max="4611" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4612" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4613" max="4613" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4614" max="4614" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4615" max="4615" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4617" max="4617" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="4618" max="4618" width="12.75" style="4" customWidth="1"/>
-    <col min="4619" max="4619" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4620" max="4620" width="14.08203125" style="4" customWidth="1"/>
-    <col min="4621" max="4621" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4622" max="4622" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4623" max="4623" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4624" max="4624" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4625" max="4625" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4626" max="4626" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4627" max="4627" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4628" max="4628" width="12.83203125" style="4" customWidth="1"/>
-    <col min="4629" max="4629" width="15.58203125" style="4" customWidth="1"/>
-    <col min="4630" max="4863" width="9" style="4"/>
-    <col min="4864" max="4864" width="37.83203125" style="4" customWidth="1"/>
-    <col min="4865" max="4865" width="6.58203125" style="4" customWidth="1"/>
-    <col min="4866" max="4866" width="9" style="4"/>
-    <col min="4867" max="4867" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4868" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4869" max="4869" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4870" max="4870" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4871" max="4871" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4873" max="4873" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="4874" max="4874" width="12.75" style="4" customWidth="1"/>
-    <col min="4875" max="4875" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4876" max="4876" width="14.08203125" style="4" customWidth="1"/>
-    <col min="4877" max="4877" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4878" max="4878" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4879" max="4879" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4880" max="4880" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4881" max="4881" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4882" max="4882" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4883" max="4883" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4884" max="4884" width="12.83203125" style="4" customWidth="1"/>
-    <col min="4885" max="4885" width="15.58203125" style="4" customWidth="1"/>
-    <col min="4886" max="5119" width="9" style="4"/>
-    <col min="5120" max="5120" width="37.83203125" style="4" customWidth="1"/>
-    <col min="5121" max="5121" width="6.58203125" style="4" customWidth="1"/>
-    <col min="5122" max="5122" width="9" style="4"/>
-    <col min="5123" max="5123" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5124" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5125" max="5125" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5126" max="5126" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5127" max="5127" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5129" max="5129" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5130" width="12.75" style="4" customWidth="1"/>
-    <col min="5131" max="5131" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5132" max="5132" width="14.08203125" style="4" customWidth="1"/>
-    <col min="5133" max="5133" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5134" max="5134" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="5135" max="5135" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="5136" max="5136" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5137" max="5137" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5138" max="5138" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5139" max="5139" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5140" max="5140" width="12.83203125" style="4" customWidth="1"/>
-    <col min="5141" max="5141" width="15.58203125" style="4" customWidth="1"/>
-    <col min="5142" max="5375" width="9" style="4"/>
-    <col min="5376" max="5376" width="37.83203125" style="4" customWidth="1"/>
-    <col min="5377" max="5377" width="6.58203125" style="4" customWidth="1"/>
-    <col min="5378" max="5378" width="9" style="4"/>
-    <col min="5379" max="5379" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5380" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5381" max="5381" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5382" max="5382" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5383" max="5383" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5385" max="5385" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5386" max="5386" width="12.75" style="4" customWidth="1"/>
-    <col min="5387" max="5387" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5388" max="5388" width="14.08203125" style="4" customWidth="1"/>
-    <col min="5389" max="5389" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5390" max="5390" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="5391" max="5391" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="5392" max="5392" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5393" max="5393" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5394" max="5394" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5395" max="5395" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5396" max="5396" width="12.83203125" style="4" customWidth="1"/>
-    <col min="5397" max="5397" width="15.58203125" style="4" customWidth="1"/>
-    <col min="5398" max="5631" width="9" style="4"/>
-    <col min="5632" max="5632" width="37.83203125" style="4" customWidth="1"/>
-    <col min="5633" max="5633" width="6.58203125" style="4" customWidth="1"/>
-    <col min="5634" max="5634" width="9" style="4"/>
-    <col min="5635" max="5635" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5636" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5637" max="5637" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5638" max="5638" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5639" max="5639" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5641" max="5641" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5642" max="5642" width="12.75" style="4" customWidth="1"/>
-    <col min="5643" max="5643" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5644" max="5644" width="14.08203125" style="4" customWidth="1"/>
-    <col min="5645" max="5645" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5646" max="5646" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5647" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="5648" max="5648" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5649" max="5649" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5650" max="5650" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5651" max="5651" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5652" max="5652" width="12.83203125" style="4" customWidth="1"/>
-    <col min="5653" max="5653" width="15.58203125" style="4" customWidth="1"/>
-    <col min="5654" max="5887" width="9" style="4"/>
-    <col min="5888" max="5888" width="37.83203125" style="4" customWidth="1"/>
-    <col min="5889" max="5889" width="6.58203125" style="4" customWidth="1"/>
-    <col min="5890" max="5890" width="9" style="4"/>
-    <col min="5891" max="5891" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5892" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5893" max="5893" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5894" max="5894" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5895" max="5895" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5897" max="5897" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5898" max="5898" width="12.75" style="4" customWidth="1"/>
-    <col min="5899" max="5899" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5900" max="5900" width="14.08203125" style="4" customWidth="1"/>
-    <col min="5901" max="5901" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5902" max="5902" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="5903" max="5903" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="5904" max="5904" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5905" max="5905" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5906" max="5906" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5907" max="5907" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5908" max="5908" width="12.83203125" style="4" customWidth="1"/>
-    <col min="5909" max="5909" width="15.58203125" style="4" customWidth="1"/>
-    <col min="5910" max="6143" width="9" style="4"/>
-    <col min="6144" max="6144" width="37.83203125" style="4" customWidth="1"/>
-    <col min="6145" max="6145" width="6.58203125" style="4" customWidth="1"/>
-    <col min="6146" max="6146" width="9" style="4"/>
-    <col min="6147" max="6147" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6148" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6149" max="6149" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6150" max="6150" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6151" max="6151" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6153" max="6153" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6154" max="6154" width="12.75" style="4" customWidth="1"/>
-    <col min="6155" max="6155" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6156" max="6156" width="14.08203125" style="4" customWidth="1"/>
-    <col min="6157" max="6157" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6158" max="6158" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="6159" max="6159" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6160" max="6160" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6161" max="6161" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6162" max="6162" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6163" max="6163" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6164" max="6164" width="12.83203125" style="4" customWidth="1"/>
-    <col min="6165" max="6165" width="15.58203125" style="4" customWidth="1"/>
-    <col min="6166" max="6399" width="9" style="4"/>
-    <col min="6400" max="6400" width="37.83203125" style="4" customWidth="1"/>
-    <col min="6401" max="6401" width="6.58203125" style="4" customWidth="1"/>
-    <col min="6402" max="6402" width="9" style="4"/>
-    <col min="6403" max="6403" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6404" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6405" max="6405" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6406" max="6406" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6407" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6409" max="6409" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6410" max="6410" width="12.75" style="4" customWidth="1"/>
-    <col min="6411" max="6411" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6412" max="6412" width="14.08203125" style="4" customWidth="1"/>
-    <col min="6413" max="6413" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6414" max="6414" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="6415" max="6415" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6416" max="6416" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6417" max="6417" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6418" max="6418" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6419" max="6419" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6420" max="6420" width="12.83203125" style="4" customWidth="1"/>
-    <col min="6421" max="6421" width="15.58203125" style="4" customWidth="1"/>
-    <col min="6422" max="6655" width="9" style="4"/>
-    <col min="6656" max="6656" width="37.83203125" style="4" customWidth="1"/>
-    <col min="6657" max="6657" width="6.58203125" style="4" customWidth="1"/>
-    <col min="6658" max="6658" width="9" style="4"/>
-    <col min="6659" max="6659" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6660" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6661" max="6661" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6662" max="6662" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6663" max="6663" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6665" max="6665" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6666" max="6666" width="12.75" style="4" customWidth="1"/>
-    <col min="6667" max="6667" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6668" max="6668" width="14.08203125" style="4" customWidth="1"/>
-    <col min="6669" max="6669" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6670" max="6670" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="6671" max="6671" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6672" max="6672" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6673" max="6673" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6674" max="6674" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6675" max="6675" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6676" max="6676" width="12.83203125" style="4" customWidth="1"/>
-    <col min="6677" max="6677" width="15.58203125" style="4" customWidth="1"/>
-    <col min="6678" max="6911" width="9" style="4"/>
-    <col min="6912" max="6912" width="37.83203125" style="4" customWidth="1"/>
-    <col min="6913" max="6913" width="6.58203125" style="4" customWidth="1"/>
-    <col min="6914" max="6914" width="9" style="4"/>
-    <col min="6915" max="6915" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6916" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6917" max="6917" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6918" max="6918" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="6919" max="6919" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6921" max="6921" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6922" max="6922" width="12.75" style="4" customWidth="1"/>
-    <col min="6923" max="6923" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6924" max="6924" width="14.08203125" style="4" customWidth="1"/>
-    <col min="6925" max="6925" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6926" max="6926" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="6927" max="6927" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6928" max="6928" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6929" max="6929" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6930" max="6930" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6931" max="6931" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6932" max="6932" width="12.83203125" style="4" customWidth="1"/>
-    <col min="6933" max="6933" width="15.58203125" style="4" customWidth="1"/>
-    <col min="6934" max="7167" width="9" style="4"/>
-    <col min="7168" max="7168" width="37.83203125" style="4" customWidth="1"/>
-    <col min="7169" max="7169" width="6.58203125" style="4" customWidth="1"/>
-    <col min="7170" max="7170" width="9" style="4"/>
-    <col min="7171" max="7171" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7172" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7173" max="7173" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7174" max="7174" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="7175" max="7175" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7177" max="7177" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7178" max="7178" width="12.75" style="4" customWidth="1"/>
-    <col min="7179" max="7179" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7180" max="7180" width="14.08203125" style="4" customWidth="1"/>
-    <col min="7181" max="7181" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7182" max="7182" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="7183" max="7183" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7184" max="7184" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7185" max="7185" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7186" max="7186" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7187" max="7187" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7188" max="7188" width="12.83203125" style="4" customWidth="1"/>
-    <col min="7189" max="7189" width="15.58203125" style="4" customWidth="1"/>
-    <col min="7190" max="7423" width="9" style="4"/>
-    <col min="7424" max="7424" width="37.83203125" style="4" customWidth="1"/>
-    <col min="7425" max="7425" width="6.58203125" style="4" customWidth="1"/>
-    <col min="7426" max="7426" width="9" style="4"/>
-    <col min="7427" max="7427" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7428" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7429" max="7429" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7430" max="7430" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="7431" max="7431" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7433" max="7433" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7434" max="7434" width="12.75" style="4" customWidth="1"/>
-    <col min="7435" max="7435" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7436" max="7436" width="14.08203125" style="4" customWidth="1"/>
-    <col min="7437" max="7437" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7438" max="7438" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="7439" max="7439" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7440" max="7440" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7441" max="7441" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7442" max="7442" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7443" max="7443" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7444" max="7444" width="12.83203125" style="4" customWidth="1"/>
-    <col min="7445" max="7445" width="15.58203125" style="4" customWidth="1"/>
-    <col min="7446" max="7679" width="9" style="4"/>
-    <col min="7680" max="7680" width="37.83203125" style="4" customWidth="1"/>
-    <col min="7681" max="7681" width="6.58203125" style="4" customWidth="1"/>
-    <col min="7682" max="7682" width="9" style="4"/>
-    <col min="7683" max="7683" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7684" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7685" max="7685" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7686" max="7686" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7687" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7689" max="7689" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7690" max="7690" width="12.75" style="4" customWidth="1"/>
-    <col min="7691" max="7691" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7692" max="7692" width="14.08203125" style="4" customWidth="1"/>
-    <col min="7693" max="7693" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7694" max="7694" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="7695" max="7695" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7696" max="7696" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7697" max="7697" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7698" max="7698" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7699" max="7699" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7700" max="7700" width="12.83203125" style="4" customWidth="1"/>
-    <col min="7701" max="7701" width="15.58203125" style="4" customWidth="1"/>
-    <col min="7702" max="7935" width="9" style="4"/>
-    <col min="7936" max="7936" width="37.83203125" style="4" customWidth="1"/>
-    <col min="7937" max="7937" width="6.58203125" style="4" customWidth="1"/>
-    <col min="7938" max="7938" width="9" style="4"/>
-    <col min="7939" max="7939" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7940" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7941" max="7941" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7942" max="7942" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="7943" max="7943" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7945" max="7945" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7946" max="7946" width="12.75" style="4" customWidth="1"/>
-    <col min="7947" max="7947" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7948" max="7948" width="14.08203125" style="4" customWidth="1"/>
-    <col min="7949" max="7949" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7950" max="7950" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="7951" max="7951" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7952" max="7952" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7953" max="7953" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7954" max="7954" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7955" max="7955" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7956" max="7956" width="12.83203125" style="4" customWidth="1"/>
-    <col min="7957" max="7957" width="15.58203125" style="4" customWidth="1"/>
-    <col min="7958" max="8191" width="9" style="4"/>
-    <col min="8192" max="8192" width="37.83203125" style="4" customWidth="1"/>
-    <col min="8193" max="8193" width="6.58203125" style="4" customWidth="1"/>
-    <col min="8194" max="8194" width="9" style="4"/>
-    <col min="8195" max="8195" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8196" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8197" max="8197" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8198" max="8198" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8199" max="8199" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8201" max="8201" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="8202" max="8202" width="12.75" style="4" customWidth="1"/>
-    <col min="8203" max="8203" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8204" max="8204" width="14.08203125" style="4" customWidth="1"/>
-    <col min="8205" max="8205" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8206" max="8206" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8207" max="8207" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8208" max="8208" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8209" max="8209" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8210" max="8210" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8211" max="8211" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8212" max="8212" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8213" max="8213" width="15.58203125" style="4" customWidth="1"/>
-    <col min="8214" max="8447" width="9" style="4"/>
-    <col min="8448" max="8448" width="37.83203125" style="4" customWidth="1"/>
-    <col min="8449" max="8449" width="6.58203125" style="4" customWidth="1"/>
-    <col min="8450" max="8450" width="9" style="4"/>
-    <col min="8451" max="8451" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8452" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8453" max="8453" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8454" max="8454" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8455" max="8455" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8457" max="8457" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="8458" max="8458" width="12.75" style="4" customWidth="1"/>
-    <col min="8459" max="8459" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8460" max="8460" width="14.08203125" style="4" customWidth="1"/>
-    <col min="8461" max="8461" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8462" max="8462" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8463" max="8463" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8464" max="8464" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8465" max="8465" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8466" max="8466" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8467" max="8467" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8468" max="8468" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8469" max="8469" width="15.58203125" style="4" customWidth="1"/>
-    <col min="8470" max="8703" width="9" style="4"/>
-    <col min="8704" max="8704" width="37.83203125" style="4" customWidth="1"/>
-    <col min="8705" max="8705" width="6.58203125" style="4" customWidth="1"/>
-    <col min="8706" max="8706" width="9" style="4"/>
-    <col min="8707" max="8707" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8708" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8709" max="8709" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8710" max="8710" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8711" max="8711" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8713" max="8713" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="8714" max="8714" width="12.75" style="4" customWidth="1"/>
-    <col min="8715" max="8715" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8716" max="8716" width="14.08203125" style="4" customWidth="1"/>
-    <col min="8717" max="8717" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8718" max="8718" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8719" max="8719" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8720" max="8720" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8721" max="8721" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8722" max="8722" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8723" max="8723" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8724" max="8724" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8725" max="8725" width="15.58203125" style="4" customWidth="1"/>
-    <col min="8726" max="8959" width="9" style="4"/>
-    <col min="8960" max="8960" width="37.83203125" style="4" customWidth="1"/>
-    <col min="8961" max="8961" width="6.58203125" style="4" customWidth="1"/>
-    <col min="8962" max="8962" width="9" style="4"/>
-    <col min="8963" max="8963" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8964" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8965" max="8965" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8966" max="8966" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8967" max="8967" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8969" max="8969" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="8970" max="8970" width="12.75" style="4" customWidth="1"/>
-    <col min="8971" max="8971" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8972" max="8972" width="14.08203125" style="4" customWidth="1"/>
-    <col min="8973" max="8973" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8974" max="8974" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8975" max="8975" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8976" max="8976" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8977" max="8977" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8978" max="8978" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8979" max="8979" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8980" max="8980" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8981" max="8981" width="15.58203125" style="4" customWidth="1"/>
-    <col min="8982" max="9215" width="9" style="4"/>
-    <col min="9216" max="9216" width="37.83203125" style="4" customWidth="1"/>
-    <col min="9217" max="9217" width="6.58203125" style="4" customWidth="1"/>
-    <col min="9218" max="9218" width="9" style="4"/>
-    <col min="9219" max="9219" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9220" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9221" max="9221" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9222" max="9222" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="9223" max="9223" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9225" max="9225" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9226" max="9226" width="12.75" style="4" customWidth="1"/>
-    <col min="9227" max="9227" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9228" max="9228" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9229" max="9229" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9230" max="9230" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="9231" max="9231" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="9232" max="9232" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9233" max="9233" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9234" max="9234" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9235" max="9235" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9236" max="9236" width="12.83203125" style="4" customWidth="1"/>
-    <col min="9237" max="9237" width="15.58203125" style="4" customWidth="1"/>
-    <col min="9238" max="9471" width="9" style="4"/>
-    <col min="9472" max="9472" width="37.83203125" style="4" customWidth="1"/>
-    <col min="9473" max="9473" width="6.58203125" style="4" customWidth="1"/>
-    <col min="9474" max="9474" width="9" style="4"/>
-    <col min="9475" max="9475" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9476" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9477" max="9477" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9478" max="9478" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="9479" max="9479" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9481" max="9481" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9482" width="12.75" style="4" customWidth="1"/>
-    <col min="9483" max="9483" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9484" max="9484" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9485" max="9485" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9486" max="9486" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="9487" max="9487" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="9488" max="9488" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9489" max="9489" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9490" max="9490" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9491" max="9491" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9492" max="9492" width="12.83203125" style="4" customWidth="1"/>
-    <col min="9493" max="9493" width="15.58203125" style="4" customWidth="1"/>
-    <col min="9494" max="9727" width="9" style="4"/>
-    <col min="9728" max="9728" width="37.83203125" style="4" customWidth="1"/>
-    <col min="9729" max="9729" width="6.58203125" style="4" customWidth="1"/>
-    <col min="9730" max="9730" width="9" style="4"/>
-    <col min="9731" max="9731" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9732" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9733" max="9733" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9734" max="9734" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="9735" max="9735" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9737" max="9737" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9738" max="9738" width="12.75" style="4" customWidth="1"/>
-    <col min="9739" max="9739" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9740" max="9740" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9741" max="9741" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9742" max="9742" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="9743" max="9743" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="9744" max="9744" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9745" max="9745" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9746" max="9746" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9747" max="9747" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9748" max="9748" width="12.83203125" style="4" customWidth="1"/>
-    <col min="9749" max="9749" width="15.58203125" style="4" customWidth="1"/>
-    <col min="9750" max="9983" width="9" style="4"/>
-    <col min="9984" max="9984" width="37.83203125" style="4" customWidth="1"/>
-    <col min="9985" max="9985" width="6.58203125" style="4" customWidth="1"/>
-    <col min="9986" max="9986" width="9" style="4"/>
-    <col min="9987" max="9987" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9988" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9989" max="9989" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9990" max="9990" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="9991" max="9991" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9993" max="9993" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9994" max="9994" width="12.75" style="4" customWidth="1"/>
-    <col min="9995" max="9995" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="9996" max="9996" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9997" max="9997" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9998" max="9998" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="9999" max="9999" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10000" max="10000" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10001" max="10001" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10002" max="10002" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10003" max="10003" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10004" max="10004" width="12.83203125" style="4" customWidth="1"/>
-    <col min="10005" max="10005" width="15.58203125" style="4" customWidth="1"/>
-    <col min="10006" max="10239" width="9" style="4"/>
-    <col min="10240" max="10240" width="37.83203125" style="4" customWidth="1"/>
-    <col min="10241" max="10241" width="6.58203125" style="4" customWidth="1"/>
-    <col min="10242" max="10242" width="9" style="4"/>
-    <col min="10243" max="10243" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10244" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10245" max="10245" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10246" max="10246" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="10247" max="10247" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10249" max="10249" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10250" max="10250" width="12.75" style="4" customWidth="1"/>
-    <col min="10251" max="10251" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10252" max="10252" width="14.08203125" style="4" customWidth="1"/>
-    <col min="10253" max="10253" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10254" max="10254" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="10255" max="10255" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10256" max="10256" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10257" max="10257" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10258" max="10258" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10259" max="10259" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10260" max="10260" width="12.83203125" style="4" customWidth="1"/>
-    <col min="10261" max="10261" width="15.58203125" style="4" customWidth="1"/>
-    <col min="10262" max="10495" width="9" style="4"/>
-    <col min="10496" max="10496" width="37.83203125" style="4" customWidth="1"/>
-    <col min="10497" max="10497" width="6.58203125" style="4" customWidth="1"/>
-    <col min="10498" max="10498" width="9" style="4"/>
-    <col min="10499" max="10499" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10500" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10501" max="10501" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10502" max="10502" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="10503" max="10503" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10505" max="10505" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10506" max="10506" width="12.75" style="4" customWidth="1"/>
-    <col min="10507" max="10507" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10508" max="10508" width="14.08203125" style="4" customWidth="1"/>
-    <col min="10509" max="10509" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10510" max="10510" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="10511" max="10511" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10512" max="10512" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10513" max="10513" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10514" max="10514" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10515" max="10515" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10516" max="10516" width="12.83203125" style="4" customWidth="1"/>
-    <col min="10517" max="10517" width="15.58203125" style="4" customWidth="1"/>
-    <col min="10518" max="10751" width="9" style="4"/>
-    <col min="10752" max="10752" width="37.83203125" style="4" customWidth="1"/>
-    <col min="10753" max="10753" width="6.58203125" style="4" customWidth="1"/>
-    <col min="10754" max="10754" width="9" style="4"/>
-    <col min="10755" max="10755" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10756" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10757" max="10757" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10758" max="10758" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="10759" max="10759" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10761" max="10761" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10762" max="10762" width="12.75" style="4" customWidth="1"/>
-    <col min="10763" max="10763" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10764" max="10764" width="14.08203125" style="4" customWidth="1"/>
-    <col min="10765" max="10765" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10766" max="10766" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="10767" max="10767" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10768" max="10768" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10769" max="10769" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10770" max="10770" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10771" max="10771" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10772" max="10772" width="12.83203125" style="4" customWidth="1"/>
-    <col min="10773" max="10773" width="15.58203125" style="4" customWidth="1"/>
-    <col min="10774" max="11007" width="9" style="4"/>
-    <col min="11008" max="11008" width="37.83203125" style="4" customWidth="1"/>
-    <col min="11009" max="11009" width="6.58203125" style="4" customWidth="1"/>
-    <col min="11010" max="11010" width="9" style="4"/>
-    <col min="11011" max="11011" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11012" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11013" max="11013" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11014" max="11014" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="11015" max="11015" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11017" max="11017" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11018" max="11018" width="12.75" style="4" customWidth="1"/>
-    <col min="11019" max="11019" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11020" max="11020" width="14.08203125" style="4" customWidth="1"/>
-    <col min="11021" max="11021" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11022" max="11022" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="11023" max="11023" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="11024" max="11024" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11025" max="11025" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11026" max="11026" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11027" max="11027" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11028" max="11028" width="12.83203125" style="4" customWidth="1"/>
-    <col min="11029" max="11029" width="15.58203125" style="4" customWidth="1"/>
-    <col min="11030" max="11263" width="9" style="4"/>
-    <col min="11264" max="11264" width="37.83203125" style="4" customWidth="1"/>
-    <col min="11265" max="11265" width="6.58203125" style="4" customWidth="1"/>
-    <col min="11266" max="11266" width="9" style="4"/>
-    <col min="11267" max="11267" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11268" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11269" max="11269" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11270" max="11270" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="11271" max="11271" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11273" max="11273" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11274" max="11274" width="12.75" style="4" customWidth="1"/>
-    <col min="11275" max="11275" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11276" max="11276" width="14.08203125" style="4" customWidth="1"/>
-    <col min="11277" max="11277" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11278" max="11278" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="11279" max="11279" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="11280" max="11280" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11281" max="11281" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11282" max="11282" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11283" max="11283" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11284" max="11284" width="12.83203125" style="4" customWidth="1"/>
-    <col min="11285" max="11285" width="15.58203125" style="4" customWidth="1"/>
-    <col min="11286" max="11519" width="9" style="4"/>
-    <col min="11520" max="11520" width="37.83203125" style="4" customWidth="1"/>
-    <col min="11521" max="11521" width="6.58203125" style="4" customWidth="1"/>
-    <col min="11522" max="11522" width="9" style="4"/>
-    <col min="11523" max="11523" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11524" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11525" max="11525" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11526" max="11526" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="11527" max="11527" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11529" max="11529" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11530" max="11530" width="12.75" style="4" customWidth="1"/>
-    <col min="11531" max="11531" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11532" max="11532" width="14.08203125" style="4" customWidth="1"/>
-    <col min="11533" max="11533" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11534" max="11534" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="11535" max="11535" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="11536" max="11536" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11537" max="11537" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11538" max="11538" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11539" max="11539" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11540" max="11540" width="12.83203125" style="4" customWidth="1"/>
-    <col min="11541" max="11541" width="15.58203125" style="4" customWidth="1"/>
-    <col min="11542" max="11775" width="9" style="4"/>
-    <col min="11776" max="11776" width="37.83203125" style="4" customWidth="1"/>
-    <col min="11777" max="11777" width="6.58203125" style="4" customWidth="1"/>
-    <col min="11778" max="11778" width="9" style="4"/>
-    <col min="11779" max="11779" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11780" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11781" max="11781" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11782" max="11782" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="11783" max="11783" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11785" max="11785" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="11786" max="11786" width="12.75" style="4" customWidth="1"/>
-    <col min="11787" max="11787" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11788" max="11788" width="14.08203125" style="4" customWidth="1"/>
-    <col min="11789" max="11789" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11790" max="11790" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="11791" max="11791" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="11792" max="11792" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11793" max="11793" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11794" max="11794" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11795" max="11795" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11796" max="11796" width="12.83203125" style="4" customWidth="1"/>
-    <col min="11797" max="11797" width="15.58203125" style="4" customWidth="1"/>
-    <col min="11798" max="12031" width="9" style="4"/>
-    <col min="12032" max="12032" width="37.83203125" style="4" customWidth="1"/>
-    <col min="12033" max="12033" width="6.58203125" style="4" customWidth="1"/>
-    <col min="12034" max="12034" width="9" style="4"/>
-    <col min="12035" max="12035" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12036" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12037" max="12037" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12038" max="12038" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12039" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12041" max="12041" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="12042" max="12042" width="12.75" style="4" customWidth="1"/>
-    <col min="12043" max="12043" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12044" max="12044" width="14.08203125" style="4" customWidth="1"/>
-    <col min="12045" max="12045" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12046" max="12046" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12047" max="12047" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="12048" max="12048" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12049" max="12049" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12050" max="12050" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12051" max="12051" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12052" max="12052" width="12.83203125" style="4" customWidth="1"/>
-    <col min="12053" max="12053" width="15.58203125" style="4" customWidth="1"/>
-    <col min="12054" max="12287" width="9" style="4"/>
-    <col min="12288" max="12288" width="37.83203125" style="4" customWidth="1"/>
-    <col min="12289" max="12289" width="6.58203125" style="4" customWidth="1"/>
-    <col min="12290" max="12290" width="9" style="4"/>
-    <col min="12291" max="12291" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12292" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12293" max="12293" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12294" max="12294" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="12295" max="12295" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12297" max="12297" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="12298" max="12298" width="12.75" style="4" customWidth="1"/>
-    <col min="12299" max="12299" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12300" max="12300" width="14.08203125" style="4" customWidth="1"/>
-    <col min="12301" max="12301" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12302" max="12302" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12303" max="12303" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="12304" max="12304" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12305" max="12305" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12306" max="12306" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12307" max="12307" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12308" max="12308" width="12.83203125" style="4" customWidth="1"/>
-    <col min="12309" max="12309" width="15.58203125" style="4" customWidth="1"/>
-    <col min="12310" max="12543" width="9" style="4"/>
-    <col min="12544" max="12544" width="37.83203125" style="4" customWidth="1"/>
-    <col min="12545" max="12545" width="6.58203125" style="4" customWidth="1"/>
-    <col min="12546" max="12546" width="9" style="4"/>
-    <col min="12547" max="12547" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12548" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12549" max="12549" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12550" max="12550" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="12551" max="12551" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12553" max="12553" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="12554" max="12554" width="12.75" style="4" customWidth="1"/>
-    <col min="12555" max="12555" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12556" max="12556" width="14.08203125" style="4" customWidth="1"/>
-    <col min="12557" max="12557" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12558" max="12558" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12559" max="12559" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="12560" max="12560" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12561" max="12561" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12562" max="12562" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12563" max="12563" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12564" max="12564" width="12.83203125" style="4" customWidth="1"/>
-    <col min="12565" max="12565" width="15.58203125" style="4" customWidth="1"/>
-    <col min="12566" max="12799" width="9" style="4"/>
-    <col min="12800" max="12800" width="37.83203125" style="4" customWidth="1"/>
-    <col min="12801" max="12801" width="6.58203125" style="4" customWidth="1"/>
-    <col min="12802" max="12802" width="9" style="4"/>
-    <col min="12803" max="12803" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12804" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12805" max="12805" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12806" max="12806" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="12807" max="12807" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12809" max="12809" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="12810" max="12810" width="12.75" style="4" customWidth="1"/>
-    <col min="12811" max="12811" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12812" max="12812" width="14.08203125" style="4" customWidth="1"/>
-    <col min="12813" max="12813" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12814" max="12814" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12815" max="12815" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="12816" max="12816" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12817" max="12817" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12818" max="12818" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12819" max="12819" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12820" max="12820" width="12.83203125" style="4" customWidth="1"/>
-    <col min="12821" max="12821" width="15.58203125" style="4" customWidth="1"/>
-    <col min="12822" max="13055" width="9" style="4"/>
-    <col min="13056" max="13056" width="37.83203125" style="4" customWidth="1"/>
-    <col min="13057" max="13057" width="6.58203125" style="4" customWidth="1"/>
-    <col min="13058" max="13058" width="9" style="4"/>
-    <col min="13059" max="13059" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13060" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13061" max="13061" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13062" max="13062" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="13063" max="13063" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13065" max="13065" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="13066" max="13066" width="12.75" style="4" customWidth="1"/>
-    <col min="13067" max="13067" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13068" max="13068" width="14.08203125" style="4" customWidth="1"/>
-    <col min="13069" max="13069" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13070" max="13070" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13071" max="13071" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="13072" max="13072" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13073" max="13073" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13074" max="13074" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13075" max="13075" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13076" max="13076" width="12.83203125" style="4" customWidth="1"/>
-    <col min="13077" max="13077" width="15.58203125" style="4" customWidth="1"/>
-    <col min="13078" max="13311" width="9" style="4"/>
-    <col min="13312" max="13312" width="37.83203125" style="4" customWidth="1"/>
-    <col min="13313" max="13313" width="6.58203125" style="4" customWidth="1"/>
-    <col min="13314" max="13314" width="9" style="4"/>
-    <col min="13315" max="13315" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13316" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13317" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13318" max="13318" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="13319" max="13319" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13321" max="13321" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="13322" max="13322" width="12.75" style="4" customWidth="1"/>
-    <col min="13323" max="13323" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13324" max="13324" width="14.08203125" style="4" customWidth="1"/>
-    <col min="13325" max="13325" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13326" max="13326" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13327" max="13327" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="13328" max="13328" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13329" max="13329" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13330" max="13330" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13331" max="13331" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13332" max="13332" width="12.83203125" style="4" customWidth="1"/>
-    <col min="13333" max="13333" width="15.58203125" style="4" customWidth="1"/>
-    <col min="13334" max="13567" width="9" style="4"/>
-    <col min="13568" max="13568" width="37.83203125" style="4" customWidth="1"/>
-    <col min="13569" max="13569" width="6.58203125" style="4" customWidth="1"/>
-    <col min="13570" max="13570" width="9" style="4"/>
-    <col min="13571" max="13571" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13572" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13573" max="13573" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13574" max="13574" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="13575" max="13575" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13577" max="13577" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="13578" max="13578" width="12.75" style="4" customWidth="1"/>
-    <col min="13579" max="13579" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13580" max="13580" width="14.08203125" style="4" customWidth="1"/>
-    <col min="13581" max="13581" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13582" max="13582" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13583" max="13583" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="13584" max="13584" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13585" max="13585" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13586" max="13586" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13587" max="13587" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13588" max="13588" width="12.83203125" style="4" customWidth="1"/>
-    <col min="13589" max="13589" width="15.58203125" style="4" customWidth="1"/>
-    <col min="13590" max="13823" width="9" style="4"/>
-    <col min="13824" max="13824" width="37.83203125" style="4" customWidth="1"/>
-    <col min="13825" max="13825" width="6.58203125" style="4" customWidth="1"/>
-    <col min="13826" max="13826" width="9" style="4"/>
-    <col min="13827" max="13827" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13828" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13829" max="13829" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13830" max="13830" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="13831" max="13831" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13833" max="13833" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="13834" max="13834" width="12.75" style="4" customWidth="1"/>
-    <col min="13835" max="13835" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13836" max="13836" width="14.08203125" style="4" customWidth="1"/>
-    <col min="13837" max="13837" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13838" max="13838" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13839" max="13839" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="13840" max="13840" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13841" max="13841" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13842" max="13842" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13843" max="13843" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13844" max="13844" width="12.83203125" style="4" customWidth="1"/>
-    <col min="13845" max="13845" width="15.58203125" style="4" customWidth="1"/>
-    <col min="13846" max="14079" width="9" style="4"/>
-    <col min="14080" max="14080" width="37.83203125" style="4" customWidth="1"/>
-    <col min="14081" max="14081" width="6.58203125" style="4" customWidth="1"/>
-    <col min="14082" max="14082" width="9" style="4"/>
-    <col min="14083" max="14083" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14084" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14085" max="14085" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14086" max="14086" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14087" max="14087" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14089" max="14089" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="14090" max="14090" width="12.75" style="4" customWidth="1"/>
-    <col min="14091" max="14091" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14092" max="14092" width="14.08203125" style="4" customWidth="1"/>
-    <col min="14093" max="14093" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14094" max="14094" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="14095" max="14095" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="14096" max="14096" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14097" max="14097" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14098" max="14098" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14099" max="14099" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14100" max="14100" width="12.83203125" style="4" customWidth="1"/>
-    <col min="14101" max="14101" width="15.58203125" style="4" customWidth="1"/>
-    <col min="14102" max="14335" width="9" style="4"/>
-    <col min="14336" max="14336" width="37.83203125" style="4" customWidth="1"/>
-    <col min="14337" max="14337" width="6.58203125" style="4" customWidth="1"/>
-    <col min="14338" max="14338" width="9" style="4"/>
-    <col min="14339" max="14339" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14340" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14341" max="14341" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14342" max="14342" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14343" max="14343" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14345" max="14345" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="14346" max="14346" width="12.75" style="4" customWidth="1"/>
-    <col min="14347" max="14347" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14348" max="14348" width="14.08203125" style="4" customWidth="1"/>
-    <col min="14349" max="14349" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14350" max="14350" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="14351" max="14351" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="14352" max="14352" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14353" max="14353" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14354" max="14354" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14355" max="14355" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14356" max="14356" width="12.83203125" style="4" customWidth="1"/>
-    <col min="14357" max="14357" width="15.58203125" style="4" customWidth="1"/>
-    <col min="14358" max="14591" width="9" style="4"/>
-    <col min="14592" max="14592" width="37.83203125" style="4" customWidth="1"/>
-    <col min="14593" max="14593" width="6.58203125" style="4" customWidth="1"/>
-    <col min="14594" max="14594" width="9" style="4"/>
-    <col min="14595" max="14595" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14596" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14597" max="14597" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14598" max="14598" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14599" max="14599" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14601" max="14601" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="14602" max="14602" width="12.75" style="4" customWidth="1"/>
-    <col min="14603" max="14603" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14604" max="14604" width="14.08203125" style="4" customWidth="1"/>
-    <col min="14605" max="14605" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14606" max="14606" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="14607" max="14607" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="14608" max="14608" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14609" max="14609" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14610" max="14610" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14611" max="14611" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14612" max="14612" width="12.83203125" style="4" customWidth="1"/>
-    <col min="14613" max="14613" width="15.58203125" style="4" customWidth="1"/>
-    <col min="14614" max="14847" width="9" style="4"/>
-    <col min="14848" max="14848" width="37.83203125" style="4" customWidth="1"/>
-    <col min="14849" max="14849" width="6.58203125" style="4" customWidth="1"/>
-    <col min="14850" max="14850" width="9" style="4"/>
-    <col min="14851" max="14851" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14852" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14853" max="14853" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14854" max="14854" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="14855" max="14855" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14857" max="14857" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="14858" max="14858" width="12.75" style="4" customWidth="1"/>
-    <col min="14859" max="14859" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14860" max="14860" width="14.08203125" style="4" customWidth="1"/>
-    <col min="14861" max="14861" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14862" max="14862" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="14863" max="14863" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="14864" max="14864" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14865" max="14865" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14866" max="14866" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14867" max="14867" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14868" max="14868" width="12.83203125" style="4" customWidth="1"/>
-    <col min="14869" max="14869" width="15.58203125" style="4" customWidth="1"/>
-    <col min="14870" max="15103" width="9" style="4"/>
-    <col min="15104" max="15104" width="37.83203125" style="4" customWidth="1"/>
-    <col min="15105" max="15105" width="6.58203125" style="4" customWidth="1"/>
-    <col min="15106" max="15106" width="9" style="4"/>
-    <col min="15107" max="15107" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15108" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15109" max="15109" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15110" max="15110" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="15111" max="15111" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15113" max="15113" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15114" max="15114" width="12.75" style="4" customWidth="1"/>
-    <col min="15115" max="15115" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15116" max="15116" width="14.08203125" style="4" customWidth="1"/>
-    <col min="15117" max="15117" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15118" max="15118" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="15119" max="15119" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15120" max="15120" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15121" max="15121" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15122" max="15122" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15123" max="15123" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15124" max="15124" width="12.83203125" style="4" customWidth="1"/>
-    <col min="15125" max="15125" width="15.58203125" style="4" customWidth="1"/>
-    <col min="15126" max="15359" width="9" style="4"/>
-    <col min="15360" max="15360" width="37.83203125" style="4" customWidth="1"/>
-    <col min="15361" max="15361" width="6.58203125" style="4" customWidth="1"/>
-    <col min="15362" max="15362" width="9" style="4"/>
-    <col min="15363" max="15363" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15364" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15365" max="15365" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15366" max="15366" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="15367" max="15367" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15369" max="15369" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15370" max="15370" width="12.75" style="4" customWidth="1"/>
-    <col min="15371" max="15371" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15372" max="15372" width="14.08203125" style="4" customWidth="1"/>
-    <col min="15373" max="15373" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15374" max="15374" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="15375" max="15375" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15376" max="15376" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15377" max="15377" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15378" max="15378" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15379" max="15379" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15380" max="15380" width="12.83203125" style="4" customWidth="1"/>
-    <col min="15381" max="15381" width="15.58203125" style="4" customWidth="1"/>
-    <col min="15382" max="15615" width="9" style="4"/>
-    <col min="15616" max="15616" width="37.83203125" style="4" customWidth="1"/>
-    <col min="15617" max="15617" width="6.58203125" style="4" customWidth="1"/>
-    <col min="15618" max="15618" width="9" style="4"/>
-    <col min="15619" max="15619" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15620" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15621" max="15621" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15622" max="15622" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="15623" max="15623" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15625" max="15625" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15626" max="15626" width="12.75" style="4" customWidth="1"/>
-    <col min="15627" max="15627" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15628" max="15628" width="14.08203125" style="4" customWidth="1"/>
-    <col min="15629" max="15629" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15630" max="15630" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="15631" max="15631" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15632" max="15632" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15633" max="15633" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15634" max="15634" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15635" max="15635" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15636" max="15636" width="12.83203125" style="4" customWidth="1"/>
-    <col min="15637" max="15637" width="15.58203125" style="4" customWidth="1"/>
-    <col min="15638" max="15871" width="9" style="4"/>
-    <col min="15872" max="15872" width="37.83203125" style="4" customWidth="1"/>
-    <col min="15873" max="15873" width="6.58203125" style="4" customWidth="1"/>
-    <col min="15874" max="15874" width="9" style="4"/>
-    <col min="15875" max="15875" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15876" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15877" max="15877" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15878" max="15878" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="15879" max="15879" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15881" max="15881" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15882" max="15882" width="12.75" style="4" customWidth="1"/>
-    <col min="15883" max="15883" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15884" max="15884" width="14.08203125" style="4" customWidth="1"/>
-    <col min="15885" max="15885" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15886" max="15886" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="15887" max="15887" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15888" max="15888" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15889" max="15889" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15890" max="15890" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15891" max="15891" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15892" max="15892" width="12.83203125" style="4" customWidth="1"/>
-    <col min="15893" max="15893" width="15.58203125" style="4" customWidth="1"/>
-    <col min="15894" max="16127" width="9" style="4"/>
-    <col min="16128" max="16128" width="37.83203125" style="4" customWidth="1"/>
-    <col min="16129" max="16129" width="6.58203125" style="4" customWidth="1"/>
-    <col min="16130" max="16130" width="9" style="4"/>
-    <col min="16131" max="16131" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16132" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16133" max="16133" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16134" max="16134" width="11.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="16135" max="16135" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16137" max="16137" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="16138" max="16138" width="12.75" style="4" customWidth="1"/>
-    <col min="16139" max="16139" width="13.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="16140" max="16140" width="14.08203125" style="4" customWidth="1"/>
-    <col min="16141" max="16141" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16142" max="16142" width="13.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="16143" max="16143" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="16144" max="16144" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16145" max="16145" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16146" max="16146" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16147" max="16147" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16148" max="16148" width="12.83203125" style="4" customWidth="1"/>
-    <col min="16149" max="16149" width="15.58203125" style="4" customWidth="1"/>
-    <col min="16150" max="16384" width="9" style="4"/>
+    <col min="22" max="196" width="9" style="4"/>
+    <col min="197" max="197" width="37.83203125" style="4" customWidth="1"/>
+    <col min="198" max="198" width="6.58203125" style="4" customWidth="1"/>
+    <col min="199" max="199" width="9" style="4"/>
+    <col min="200" max="200" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="12.75" style="4" customWidth="1"/>
+    <col min="208" max="208" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="14.08203125" style="4" customWidth="1"/>
+    <col min="210" max="210" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="12.83203125" style="4" customWidth="1"/>
+    <col min="218" max="218" width="15.58203125" style="4" customWidth="1"/>
+    <col min="219" max="452" width="9" style="4"/>
+    <col min="453" max="453" width="37.83203125" style="4" customWidth="1"/>
+    <col min="454" max="454" width="6.58203125" style="4" customWidth="1"/>
+    <col min="455" max="455" width="9" style="4"/>
+    <col min="456" max="456" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="457" max="457" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="458" max="458" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="459" max="459" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="460" max="460" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="461" max="461" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="462" max="462" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="463" max="463" width="12.75" style="4" customWidth="1"/>
+    <col min="464" max="464" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="465" max="465" width="14.08203125" style="4" customWidth="1"/>
+    <col min="466" max="466" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="467" max="467" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="468" max="468" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="469" max="469" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="470" max="470" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="471" max="471" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="472" max="472" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="473" max="473" width="12.83203125" style="4" customWidth="1"/>
+    <col min="474" max="474" width="15.58203125" style="4" customWidth="1"/>
+    <col min="475" max="708" width="9" style="4"/>
+    <col min="709" max="709" width="37.83203125" style="4" customWidth="1"/>
+    <col min="710" max="710" width="6.58203125" style="4" customWidth="1"/>
+    <col min="711" max="711" width="9" style="4"/>
+    <col min="712" max="712" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="713" max="713" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="714" max="714" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="715" max="715" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="716" max="716" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="717" max="717" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="718" max="718" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="719" max="719" width="12.75" style="4" customWidth="1"/>
+    <col min="720" max="720" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="721" max="721" width="14.08203125" style="4" customWidth="1"/>
+    <col min="722" max="722" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="723" max="723" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="724" max="724" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="725" max="725" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="726" max="726" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="727" max="727" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="728" max="728" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="729" max="729" width="12.83203125" style="4" customWidth="1"/>
+    <col min="730" max="730" width="15.58203125" style="4" customWidth="1"/>
+    <col min="731" max="964" width="9" style="4"/>
+    <col min="965" max="965" width="37.83203125" style="4" customWidth="1"/>
+    <col min="966" max="966" width="6.58203125" style="4" customWidth="1"/>
+    <col min="967" max="967" width="9" style="4"/>
+    <col min="968" max="968" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="969" max="969" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="970" max="970" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="971" max="971" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="972" max="972" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="973" max="973" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="974" max="974" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="975" max="975" width="12.75" style="4" customWidth="1"/>
+    <col min="976" max="976" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="977" max="977" width="14.08203125" style="4" customWidth="1"/>
+    <col min="978" max="978" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="979" max="979" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="980" max="980" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="981" max="981" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="982" max="982" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="983" max="983" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="984" max="984" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="985" max="985" width="12.83203125" style="4" customWidth="1"/>
+    <col min="986" max="986" width="15.58203125" style="4" customWidth="1"/>
+    <col min="987" max="1220" width="9" style="4"/>
+    <col min="1221" max="1221" width="37.83203125" style="4" customWidth="1"/>
+    <col min="1222" max="1222" width="6.58203125" style="4" customWidth="1"/>
+    <col min="1223" max="1223" width="9" style="4"/>
+    <col min="1224" max="1224" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1225" max="1225" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1226" max="1226" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1227" max="1227" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="1228" max="1228" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1229" max="1229" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1230" max="1230" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="1231" max="1231" width="12.75" style="4" customWidth="1"/>
+    <col min="1232" max="1232" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1233" max="1233" width="14.08203125" style="4" customWidth="1"/>
+    <col min="1234" max="1234" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1235" max="1235" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1236" max="1236" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1237" max="1237" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1238" max="1238" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1239" max="1239" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1240" max="1240" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1241" max="1241" width="12.83203125" style="4" customWidth="1"/>
+    <col min="1242" max="1242" width="15.58203125" style="4" customWidth="1"/>
+    <col min="1243" max="1476" width="9" style="4"/>
+    <col min="1477" max="1477" width="37.83203125" style="4" customWidth="1"/>
+    <col min="1478" max="1478" width="6.58203125" style="4" customWidth="1"/>
+    <col min="1479" max="1479" width="9" style="4"/>
+    <col min="1480" max="1480" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1481" max="1481" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1482" max="1482" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1483" max="1483" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="1484" max="1484" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1485" max="1485" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1486" max="1486" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="1487" max="1487" width="12.75" style="4" customWidth="1"/>
+    <col min="1488" max="1488" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1489" max="1489" width="14.08203125" style="4" customWidth="1"/>
+    <col min="1490" max="1490" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1491" max="1491" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1492" max="1492" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1493" max="1493" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1494" max="1494" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1495" max="1495" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1496" max="1496" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1497" max="1497" width="12.83203125" style="4" customWidth="1"/>
+    <col min="1498" max="1498" width="15.58203125" style="4" customWidth="1"/>
+    <col min="1499" max="1732" width="9" style="4"/>
+    <col min="1733" max="1733" width="37.83203125" style="4" customWidth="1"/>
+    <col min="1734" max="1734" width="6.58203125" style="4" customWidth="1"/>
+    <col min="1735" max="1735" width="9" style="4"/>
+    <col min="1736" max="1736" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1737" max="1737" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1738" max="1738" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1739" max="1739" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="1740" max="1740" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1741" max="1741" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1742" max="1742" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="1743" max="1743" width="12.75" style="4" customWidth="1"/>
+    <col min="1744" max="1744" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1745" max="1745" width="14.08203125" style="4" customWidth="1"/>
+    <col min="1746" max="1746" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1747" max="1747" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1748" max="1748" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1749" max="1749" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1750" max="1750" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1751" max="1751" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1752" max="1752" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1753" max="1753" width="12.83203125" style="4" customWidth="1"/>
+    <col min="1754" max="1754" width="15.58203125" style="4" customWidth="1"/>
+    <col min="1755" max="1988" width="9" style="4"/>
+    <col min="1989" max="1989" width="37.83203125" style="4" customWidth="1"/>
+    <col min="1990" max="1990" width="6.58203125" style="4" customWidth="1"/>
+    <col min="1991" max="1991" width="9" style="4"/>
+    <col min="1992" max="1992" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1993" max="1993" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1994" max="1994" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1995" max="1995" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="1996" max="1996" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1997" max="1997" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1998" max="1998" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="1999" max="1999" width="12.75" style="4" customWidth="1"/>
+    <col min="2000" max="2000" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2001" max="2001" width="14.08203125" style="4" customWidth="1"/>
+    <col min="2002" max="2002" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2003" max="2003" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2004" max="2004" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="2005" max="2005" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2006" max="2006" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2007" max="2007" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2008" max="2008" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2009" max="2009" width="12.83203125" style="4" customWidth="1"/>
+    <col min="2010" max="2010" width="15.58203125" style="4" customWidth="1"/>
+    <col min="2011" max="2244" width="9" style="4"/>
+    <col min="2245" max="2245" width="37.83203125" style="4" customWidth="1"/>
+    <col min="2246" max="2246" width="6.58203125" style="4" customWidth="1"/>
+    <col min="2247" max="2247" width="9" style="4"/>
+    <col min="2248" max="2248" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2249" max="2249" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2250" max="2250" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2251" max="2251" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2252" max="2252" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2253" max="2253" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2254" max="2254" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="2255" max="2255" width="12.75" style="4" customWidth="1"/>
+    <col min="2256" max="2256" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2257" max="2257" width="14.08203125" style="4" customWidth="1"/>
+    <col min="2258" max="2258" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2259" max="2259" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2260" max="2260" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="2261" max="2261" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2262" max="2262" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2263" max="2263" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2264" max="2264" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2265" max="2265" width="12.83203125" style="4" customWidth="1"/>
+    <col min="2266" max="2266" width="15.58203125" style="4" customWidth="1"/>
+    <col min="2267" max="2500" width="9" style="4"/>
+    <col min="2501" max="2501" width="37.83203125" style="4" customWidth="1"/>
+    <col min="2502" max="2502" width="6.58203125" style="4" customWidth="1"/>
+    <col min="2503" max="2503" width="9" style="4"/>
+    <col min="2504" max="2504" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2505" max="2505" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2506" max="2506" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2507" max="2507" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2508" max="2508" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2509" max="2509" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2510" max="2510" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="2511" max="2511" width="12.75" style="4" customWidth="1"/>
+    <col min="2512" max="2512" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2513" max="2513" width="14.08203125" style="4" customWidth="1"/>
+    <col min="2514" max="2514" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2515" max="2515" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2516" max="2516" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="2517" max="2517" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2518" max="2518" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2519" max="2519" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2520" max="2520" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2521" max="2521" width="12.83203125" style="4" customWidth="1"/>
+    <col min="2522" max="2522" width="15.58203125" style="4" customWidth="1"/>
+    <col min="2523" max="2756" width="9" style="4"/>
+    <col min="2757" max="2757" width="37.83203125" style="4" customWidth="1"/>
+    <col min="2758" max="2758" width="6.58203125" style="4" customWidth="1"/>
+    <col min="2759" max="2759" width="9" style="4"/>
+    <col min="2760" max="2760" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2761" max="2761" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2762" max="2762" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2763" max="2763" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="2764" max="2764" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2765" max="2765" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2766" max="2766" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="2767" max="2767" width="12.75" style="4" customWidth="1"/>
+    <col min="2768" max="2768" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2769" max="2769" width="14.08203125" style="4" customWidth="1"/>
+    <col min="2770" max="2770" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2771" max="2771" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2772" max="2772" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="2773" max="2773" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2774" max="2774" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2775" max="2775" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2776" max="2776" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2777" max="2777" width="12.83203125" style="4" customWidth="1"/>
+    <col min="2778" max="2778" width="15.58203125" style="4" customWidth="1"/>
+    <col min="2779" max="3012" width="9" style="4"/>
+    <col min="3013" max="3013" width="37.83203125" style="4" customWidth="1"/>
+    <col min="3014" max="3014" width="6.58203125" style="4" customWidth="1"/>
+    <col min="3015" max="3015" width="9" style="4"/>
+    <col min="3016" max="3016" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3017" max="3017" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3018" max="3018" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3019" max="3019" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3020" max="3020" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3021" max="3021" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3022" max="3022" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="3023" max="3023" width="12.75" style="4" customWidth="1"/>
+    <col min="3024" max="3024" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3025" max="3025" width="14.08203125" style="4" customWidth="1"/>
+    <col min="3026" max="3026" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3027" max="3027" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3028" max="3028" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="3029" max="3029" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3030" max="3030" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3031" max="3031" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3032" max="3032" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3033" max="3033" width="12.83203125" style="4" customWidth="1"/>
+    <col min="3034" max="3034" width="15.58203125" style="4" customWidth="1"/>
+    <col min="3035" max="3268" width="9" style="4"/>
+    <col min="3269" max="3269" width="37.83203125" style="4" customWidth="1"/>
+    <col min="3270" max="3270" width="6.58203125" style="4" customWidth="1"/>
+    <col min="3271" max="3271" width="9" style="4"/>
+    <col min="3272" max="3272" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3273" max="3273" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3274" max="3274" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3275" max="3275" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3276" max="3276" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3277" max="3277" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3278" max="3278" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="3279" max="3279" width="12.75" style="4" customWidth="1"/>
+    <col min="3280" max="3280" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3281" max="3281" width="14.08203125" style="4" customWidth="1"/>
+    <col min="3282" max="3282" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3283" max="3283" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3284" max="3284" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="3285" max="3285" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3286" max="3286" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3287" max="3287" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3288" max="3288" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3289" max="3289" width="12.83203125" style="4" customWidth="1"/>
+    <col min="3290" max="3290" width="15.58203125" style="4" customWidth="1"/>
+    <col min="3291" max="3524" width="9" style="4"/>
+    <col min="3525" max="3525" width="37.83203125" style="4" customWidth="1"/>
+    <col min="3526" max="3526" width="6.58203125" style="4" customWidth="1"/>
+    <col min="3527" max="3527" width="9" style="4"/>
+    <col min="3528" max="3528" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3529" max="3529" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3530" max="3530" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3531" max="3531" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3532" max="3532" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3533" max="3533" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3534" max="3534" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="3535" max="3535" width="12.75" style="4" customWidth="1"/>
+    <col min="3536" max="3536" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3537" max="3537" width="14.08203125" style="4" customWidth="1"/>
+    <col min="3538" max="3538" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3539" max="3539" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3540" max="3540" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="3541" max="3541" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3542" max="3542" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3543" max="3543" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3544" max="3544" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3545" max="3545" width="12.83203125" style="4" customWidth="1"/>
+    <col min="3546" max="3546" width="15.58203125" style="4" customWidth="1"/>
+    <col min="3547" max="3780" width="9" style="4"/>
+    <col min="3781" max="3781" width="37.83203125" style="4" customWidth="1"/>
+    <col min="3782" max="3782" width="6.58203125" style="4" customWidth="1"/>
+    <col min="3783" max="3783" width="9" style="4"/>
+    <col min="3784" max="3784" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3785" max="3785" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3786" max="3786" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3787" max="3787" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3788" max="3788" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3789" max="3789" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3790" max="3790" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="3791" max="3791" width="12.75" style="4" customWidth="1"/>
+    <col min="3792" max="3792" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3793" max="3793" width="14.08203125" style="4" customWidth="1"/>
+    <col min="3794" max="3794" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3795" max="3795" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3796" max="3796" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="3797" max="3797" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3798" max="3798" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3799" max="3799" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3800" max="3800" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3801" max="3801" width="12.83203125" style="4" customWidth="1"/>
+    <col min="3802" max="3802" width="15.58203125" style="4" customWidth="1"/>
+    <col min="3803" max="4036" width="9" style="4"/>
+    <col min="4037" max="4037" width="37.83203125" style="4" customWidth="1"/>
+    <col min="4038" max="4038" width="6.58203125" style="4" customWidth="1"/>
+    <col min="4039" max="4039" width="9" style="4"/>
+    <col min="4040" max="4040" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4041" max="4041" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4042" max="4042" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4043" max="4043" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4044" max="4044" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4045" max="4045" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4046" max="4046" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="4047" max="4047" width="12.75" style="4" customWidth="1"/>
+    <col min="4048" max="4048" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4049" max="4049" width="14.08203125" style="4" customWidth="1"/>
+    <col min="4050" max="4050" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4051" max="4051" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="4052" max="4052" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4053" max="4053" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4054" max="4054" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4055" max="4055" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4056" max="4056" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4057" max="4057" width="12.83203125" style="4" customWidth="1"/>
+    <col min="4058" max="4058" width="15.58203125" style="4" customWidth="1"/>
+    <col min="4059" max="4292" width="9" style="4"/>
+    <col min="4293" max="4293" width="37.83203125" style="4" customWidth="1"/>
+    <col min="4294" max="4294" width="6.58203125" style="4" customWidth="1"/>
+    <col min="4295" max="4295" width="9" style="4"/>
+    <col min="4296" max="4296" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4297" max="4297" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4298" max="4298" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4299" max="4299" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4300" max="4300" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4301" max="4301" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4302" max="4302" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="4303" max="4303" width="12.75" style="4" customWidth="1"/>
+    <col min="4304" max="4304" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4305" max="4305" width="14.08203125" style="4" customWidth="1"/>
+    <col min="4306" max="4306" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4307" max="4307" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="4308" max="4308" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4309" max="4309" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4310" max="4310" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4311" max="4311" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4312" max="4312" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4313" max="4313" width="12.83203125" style="4" customWidth="1"/>
+    <col min="4314" max="4314" width="15.58203125" style="4" customWidth="1"/>
+    <col min="4315" max="4548" width="9" style="4"/>
+    <col min="4549" max="4549" width="37.83203125" style="4" customWidth="1"/>
+    <col min="4550" max="4550" width="6.58203125" style="4" customWidth="1"/>
+    <col min="4551" max="4551" width="9" style="4"/>
+    <col min="4552" max="4552" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4553" max="4553" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4554" max="4554" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4555" max="4555" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4556" max="4556" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4557" max="4557" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4558" max="4558" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="4559" max="4559" width="12.75" style="4" customWidth="1"/>
+    <col min="4560" max="4560" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4561" max="4561" width="14.08203125" style="4" customWidth="1"/>
+    <col min="4562" max="4562" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4563" max="4563" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="4564" max="4564" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4565" max="4565" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4566" max="4566" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4567" max="4567" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4568" max="4568" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4569" max="4569" width="12.83203125" style="4" customWidth="1"/>
+    <col min="4570" max="4570" width="15.58203125" style="4" customWidth="1"/>
+    <col min="4571" max="4804" width="9" style="4"/>
+    <col min="4805" max="4805" width="37.83203125" style="4" customWidth="1"/>
+    <col min="4806" max="4806" width="6.58203125" style="4" customWidth="1"/>
+    <col min="4807" max="4807" width="9" style="4"/>
+    <col min="4808" max="4808" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4809" max="4809" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4810" max="4810" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4811" max="4811" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4812" max="4812" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4813" max="4813" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4814" max="4814" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="4815" max="4815" width="12.75" style="4" customWidth="1"/>
+    <col min="4816" max="4816" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4817" max="4817" width="14.08203125" style="4" customWidth="1"/>
+    <col min="4818" max="4818" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4819" max="4819" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="4820" max="4820" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="4821" max="4821" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4822" max="4822" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4823" max="4823" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4824" max="4824" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4825" max="4825" width="12.83203125" style="4" customWidth="1"/>
+    <col min="4826" max="4826" width="15.58203125" style="4" customWidth="1"/>
+    <col min="4827" max="5060" width="9" style="4"/>
+    <col min="5061" max="5061" width="37.83203125" style="4" customWidth="1"/>
+    <col min="5062" max="5062" width="6.58203125" style="4" customWidth="1"/>
+    <col min="5063" max="5063" width="9" style="4"/>
+    <col min="5064" max="5064" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5065" max="5065" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5066" max="5066" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5067" max="5067" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5068" max="5068" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5069" max="5069" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5070" max="5070" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5071" max="5071" width="12.75" style="4" customWidth="1"/>
+    <col min="5072" max="5072" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5073" max="5073" width="14.08203125" style="4" customWidth="1"/>
+    <col min="5074" max="5074" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5075" max="5075" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="5076" max="5076" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="5077" max="5077" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5078" max="5078" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5079" max="5079" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5080" max="5080" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5081" max="5081" width="12.83203125" style="4" customWidth="1"/>
+    <col min="5082" max="5082" width="15.58203125" style="4" customWidth="1"/>
+    <col min="5083" max="5316" width="9" style="4"/>
+    <col min="5317" max="5317" width="37.83203125" style="4" customWidth="1"/>
+    <col min="5318" max="5318" width="6.58203125" style="4" customWidth="1"/>
+    <col min="5319" max="5319" width="9" style="4"/>
+    <col min="5320" max="5320" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5321" max="5321" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5322" max="5322" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5323" max="5323" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5324" max="5324" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5325" max="5325" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5326" max="5326" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5327" max="5327" width="12.75" style="4" customWidth="1"/>
+    <col min="5328" max="5328" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5329" max="5329" width="14.08203125" style="4" customWidth="1"/>
+    <col min="5330" max="5330" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5331" max="5331" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="5332" max="5332" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="5333" max="5333" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5334" max="5334" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5335" max="5335" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5336" max="5336" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5337" max="5337" width="12.83203125" style="4" customWidth="1"/>
+    <col min="5338" max="5338" width="15.58203125" style="4" customWidth="1"/>
+    <col min="5339" max="5572" width="9" style="4"/>
+    <col min="5573" max="5573" width="37.83203125" style="4" customWidth="1"/>
+    <col min="5574" max="5574" width="6.58203125" style="4" customWidth="1"/>
+    <col min="5575" max="5575" width="9" style="4"/>
+    <col min="5576" max="5576" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5577" max="5577" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5578" max="5578" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5579" max="5579" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5580" max="5580" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5581" max="5581" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5582" max="5582" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5583" max="5583" width="12.75" style="4" customWidth="1"/>
+    <col min="5584" max="5584" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5585" max="5585" width="14.08203125" style="4" customWidth="1"/>
+    <col min="5586" max="5586" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5587" max="5587" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="5588" max="5588" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="5589" max="5589" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5590" max="5590" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5591" max="5591" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5592" max="5592" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5593" max="5593" width="12.83203125" style="4" customWidth="1"/>
+    <col min="5594" max="5594" width="15.58203125" style="4" customWidth="1"/>
+    <col min="5595" max="5828" width="9" style="4"/>
+    <col min="5829" max="5829" width="37.83203125" style="4" customWidth="1"/>
+    <col min="5830" max="5830" width="6.58203125" style="4" customWidth="1"/>
+    <col min="5831" max="5831" width="9" style="4"/>
+    <col min="5832" max="5832" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5833" max="5833" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5834" max="5834" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5835" max="5835" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5836" max="5836" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5837" max="5837" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5838" max="5838" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5839" max="5839" width="12.75" style="4" customWidth="1"/>
+    <col min="5840" max="5840" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5841" max="5841" width="14.08203125" style="4" customWidth="1"/>
+    <col min="5842" max="5842" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5843" max="5843" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="5844" max="5844" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="5845" max="5845" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5846" max="5846" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5847" max="5847" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5848" max="5848" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5849" max="5849" width="12.83203125" style="4" customWidth="1"/>
+    <col min="5850" max="5850" width="15.58203125" style="4" customWidth="1"/>
+    <col min="5851" max="6084" width="9" style="4"/>
+    <col min="6085" max="6085" width="37.83203125" style="4" customWidth="1"/>
+    <col min="6086" max="6086" width="6.58203125" style="4" customWidth="1"/>
+    <col min="6087" max="6087" width="9" style="4"/>
+    <col min="6088" max="6088" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6089" max="6089" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6090" max="6090" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6091" max="6091" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="6092" max="6092" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6093" max="6093" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6094" max="6094" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="6095" max="6095" width="12.75" style="4" customWidth="1"/>
+    <col min="6096" max="6096" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6097" max="6097" width="14.08203125" style="4" customWidth="1"/>
+    <col min="6098" max="6098" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6099" max="6099" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="6100" max="6100" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6101" max="6101" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6102" max="6102" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6103" max="6103" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6104" max="6104" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6105" max="6105" width="12.83203125" style="4" customWidth="1"/>
+    <col min="6106" max="6106" width="15.58203125" style="4" customWidth="1"/>
+    <col min="6107" max="6340" width="9" style="4"/>
+    <col min="6341" max="6341" width="37.83203125" style="4" customWidth="1"/>
+    <col min="6342" max="6342" width="6.58203125" style="4" customWidth="1"/>
+    <col min="6343" max="6343" width="9" style="4"/>
+    <col min="6344" max="6344" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6345" max="6345" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6346" max="6346" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6347" max="6347" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="6348" max="6348" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6349" max="6349" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6350" max="6350" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="6351" max="6351" width="12.75" style="4" customWidth="1"/>
+    <col min="6352" max="6352" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6353" max="6353" width="14.08203125" style="4" customWidth="1"/>
+    <col min="6354" max="6354" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6355" max="6355" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="6356" max="6356" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6357" max="6357" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6358" max="6358" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6359" max="6359" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6360" max="6360" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6361" max="6361" width="12.83203125" style="4" customWidth="1"/>
+    <col min="6362" max="6362" width="15.58203125" style="4" customWidth="1"/>
+    <col min="6363" max="6596" width="9" style="4"/>
+    <col min="6597" max="6597" width="37.83203125" style="4" customWidth="1"/>
+    <col min="6598" max="6598" width="6.58203125" style="4" customWidth="1"/>
+    <col min="6599" max="6599" width="9" style="4"/>
+    <col min="6600" max="6600" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6601" max="6601" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6602" max="6602" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6603" max="6603" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="6604" max="6604" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6605" max="6605" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6606" max="6606" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="6607" max="6607" width="12.75" style="4" customWidth="1"/>
+    <col min="6608" max="6608" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6609" max="6609" width="14.08203125" style="4" customWidth="1"/>
+    <col min="6610" max="6610" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6611" max="6611" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="6612" max="6612" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6613" max="6613" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6614" max="6614" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6615" max="6615" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6616" max="6616" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6617" max="6617" width="12.83203125" style="4" customWidth="1"/>
+    <col min="6618" max="6618" width="15.58203125" style="4" customWidth="1"/>
+    <col min="6619" max="6852" width="9" style="4"/>
+    <col min="6853" max="6853" width="37.83203125" style="4" customWidth="1"/>
+    <col min="6854" max="6854" width="6.58203125" style="4" customWidth="1"/>
+    <col min="6855" max="6855" width="9" style="4"/>
+    <col min="6856" max="6856" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6857" max="6857" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6858" max="6858" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6859" max="6859" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="6860" max="6860" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6861" max="6861" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6862" max="6862" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="6863" max="6863" width="12.75" style="4" customWidth="1"/>
+    <col min="6864" max="6864" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6865" max="6865" width="14.08203125" style="4" customWidth="1"/>
+    <col min="6866" max="6866" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6867" max="6867" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="6868" max="6868" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6869" max="6869" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6870" max="6870" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6871" max="6871" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6872" max="6872" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6873" max="6873" width="12.83203125" style="4" customWidth="1"/>
+    <col min="6874" max="6874" width="15.58203125" style="4" customWidth="1"/>
+    <col min="6875" max="7108" width="9" style="4"/>
+    <col min="7109" max="7109" width="37.83203125" style="4" customWidth="1"/>
+    <col min="7110" max="7110" width="6.58203125" style="4" customWidth="1"/>
+    <col min="7111" max="7111" width="9" style="4"/>
+    <col min="7112" max="7112" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7113" max="7113" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7114" max="7114" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7115" max="7115" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="7116" max="7116" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7117" max="7117" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7118" max="7118" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7119" max="7119" width="12.75" style="4" customWidth="1"/>
+    <col min="7120" max="7120" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7121" max="7121" width="14.08203125" style="4" customWidth="1"/>
+    <col min="7122" max="7122" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7123" max="7123" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7124" max="7124" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="7125" max="7125" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7126" max="7126" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7127" max="7127" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7128" max="7128" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7129" max="7129" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7130" max="7130" width="15.58203125" style="4" customWidth="1"/>
+    <col min="7131" max="7364" width="9" style="4"/>
+    <col min="7365" max="7365" width="37.83203125" style="4" customWidth="1"/>
+    <col min="7366" max="7366" width="6.58203125" style="4" customWidth="1"/>
+    <col min="7367" max="7367" width="9" style="4"/>
+    <col min="7368" max="7368" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7369" max="7369" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7370" max="7370" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7371" max="7371" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="7372" max="7372" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7373" max="7373" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7374" max="7374" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7375" max="7375" width="12.75" style="4" customWidth="1"/>
+    <col min="7376" max="7376" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7377" max="7377" width="14.08203125" style="4" customWidth="1"/>
+    <col min="7378" max="7378" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7379" max="7379" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7380" max="7380" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="7381" max="7381" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7382" max="7382" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7383" max="7383" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7384" max="7384" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7385" max="7385" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7386" max="7386" width="15.58203125" style="4" customWidth="1"/>
+    <col min="7387" max="7620" width="9" style="4"/>
+    <col min="7621" max="7621" width="37.83203125" style="4" customWidth="1"/>
+    <col min="7622" max="7622" width="6.58203125" style="4" customWidth="1"/>
+    <col min="7623" max="7623" width="9" style="4"/>
+    <col min="7624" max="7624" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7625" max="7625" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7626" max="7626" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7627" max="7627" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="7628" max="7628" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7629" max="7629" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7630" max="7630" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7631" max="7631" width="12.75" style="4" customWidth="1"/>
+    <col min="7632" max="7632" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7633" max="7633" width="14.08203125" style="4" customWidth="1"/>
+    <col min="7634" max="7634" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7635" max="7635" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7636" max="7636" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="7637" max="7637" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7638" max="7638" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7639" max="7639" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7640" max="7640" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7641" max="7641" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7642" max="7642" width="15.58203125" style="4" customWidth="1"/>
+    <col min="7643" max="7876" width="9" style="4"/>
+    <col min="7877" max="7877" width="37.83203125" style="4" customWidth="1"/>
+    <col min="7878" max="7878" width="6.58203125" style="4" customWidth="1"/>
+    <col min="7879" max="7879" width="9" style="4"/>
+    <col min="7880" max="7880" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7881" max="7881" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7882" max="7882" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7883" max="7883" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="7884" max="7884" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7885" max="7885" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7886" max="7886" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7887" max="7887" width="12.75" style="4" customWidth="1"/>
+    <col min="7888" max="7888" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7889" max="7889" width="14.08203125" style="4" customWidth="1"/>
+    <col min="7890" max="7890" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7891" max="7891" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7892" max="7892" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="7893" max="7893" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7894" max="7894" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7895" max="7895" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7896" max="7896" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7897" max="7897" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7898" max="7898" width="15.58203125" style="4" customWidth="1"/>
+    <col min="7899" max="8132" width="9" style="4"/>
+    <col min="8133" max="8133" width="37.83203125" style="4" customWidth="1"/>
+    <col min="8134" max="8134" width="6.58203125" style="4" customWidth="1"/>
+    <col min="8135" max="8135" width="9" style="4"/>
+    <col min="8136" max="8136" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8137" max="8137" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8138" max="8138" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8139" max="8139" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="8140" max="8140" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8141" max="8141" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8142" max="8142" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="8143" max="8143" width="12.75" style="4" customWidth="1"/>
+    <col min="8144" max="8144" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8145" max="8145" width="14.08203125" style="4" customWidth="1"/>
+    <col min="8146" max="8146" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8147" max="8147" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="8148" max="8148" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="8149" max="8149" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8150" max="8150" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8151" max="8151" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8152" max="8152" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8153" max="8153" width="12.83203125" style="4" customWidth="1"/>
+    <col min="8154" max="8154" width="15.58203125" style="4" customWidth="1"/>
+    <col min="8155" max="8388" width="9" style="4"/>
+    <col min="8389" max="8389" width="37.83203125" style="4" customWidth="1"/>
+    <col min="8390" max="8390" width="6.58203125" style="4" customWidth="1"/>
+    <col min="8391" max="8391" width="9" style="4"/>
+    <col min="8392" max="8392" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8393" max="8393" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8394" max="8394" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8395" max="8395" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="8396" max="8396" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8397" max="8397" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8398" max="8398" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="8399" max="8399" width="12.75" style="4" customWidth="1"/>
+    <col min="8400" max="8400" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8401" max="8401" width="14.08203125" style="4" customWidth="1"/>
+    <col min="8402" max="8402" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8403" max="8403" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="8404" max="8404" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="8405" max="8405" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8406" max="8406" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8407" max="8407" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8408" max="8408" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8409" max="8409" width="12.83203125" style="4" customWidth="1"/>
+    <col min="8410" max="8410" width="15.58203125" style="4" customWidth="1"/>
+    <col min="8411" max="8644" width="9" style="4"/>
+    <col min="8645" max="8645" width="37.83203125" style="4" customWidth="1"/>
+    <col min="8646" max="8646" width="6.58203125" style="4" customWidth="1"/>
+    <col min="8647" max="8647" width="9" style="4"/>
+    <col min="8648" max="8648" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8649" max="8649" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8650" max="8650" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8651" max="8651" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="8652" max="8652" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8653" max="8653" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8654" max="8654" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="8655" max="8655" width="12.75" style="4" customWidth="1"/>
+    <col min="8656" max="8656" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8657" max="8657" width="14.08203125" style="4" customWidth="1"/>
+    <col min="8658" max="8658" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8659" max="8659" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="8660" max="8660" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="8661" max="8661" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8662" max="8662" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8663" max="8663" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8664" max="8664" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8665" max="8665" width="12.83203125" style="4" customWidth="1"/>
+    <col min="8666" max="8666" width="15.58203125" style="4" customWidth="1"/>
+    <col min="8667" max="8900" width="9" style="4"/>
+    <col min="8901" max="8901" width="37.83203125" style="4" customWidth="1"/>
+    <col min="8902" max="8902" width="6.58203125" style="4" customWidth="1"/>
+    <col min="8903" max="8903" width="9" style="4"/>
+    <col min="8904" max="8904" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8905" max="8905" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8906" max="8906" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8907" max="8907" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="8908" max="8908" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8909" max="8909" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8910" max="8910" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="8911" max="8911" width="12.75" style="4" customWidth="1"/>
+    <col min="8912" max="8912" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8913" max="8913" width="14.08203125" style="4" customWidth="1"/>
+    <col min="8914" max="8914" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8915" max="8915" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="8916" max="8916" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="8917" max="8917" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8918" max="8918" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8919" max="8919" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8920" max="8920" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8921" max="8921" width="12.83203125" style="4" customWidth="1"/>
+    <col min="8922" max="8922" width="15.58203125" style="4" customWidth="1"/>
+    <col min="8923" max="9156" width="9" style="4"/>
+    <col min="9157" max="9157" width="37.83203125" style="4" customWidth="1"/>
+    <col min="9158" max="9158" width="6.58203125" style="4" customWidth="1"/>
+    <col min="9159" max="9159" width="9" style="4"/>
+    <col min="9160" max="9160" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9161" max="9161" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9162" max="9162" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9163" max="9163" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9164" max="9164" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9165" max="9165" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9166" max="9166" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="9167" max="9167" width="12.75" style="4" customWidth="1"/>
+    <col min="9168" max="9168" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9169" max="9169" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9170" max="9170" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9171" max="9171" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="9172" max="9172" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="9173" max="9173" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9174" max="9174" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9175" max="9175" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9176" max="9176" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9177" max="9177" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9178" max="9178" width="15.58203125" style="4" customWidth="1"/>
+    <col min="9179" max="9412" width="9" style="4"/>
+    <col min="9413" max="9413" width="37.83203125" style="4" customWidth="1"/>
+    <col min="9414" max="9414" width="6.58203125" style="4" customWidth="1"/>
+    <col min="9415" max="9415" width="9" style="4"/>
+    <col min="9416" max="9416" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9417" max="9417" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9418" max="9418" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9419" max="9419" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9420" max="9420" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9421" max="9421" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9422" max="9422" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="9423" max="9423" width="12.75" style="4" customWidth="1"/>
+    <col min="9424" max="9424" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9425" max="9425" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9426" max="9426" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9427" max="9427" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="9428" max="9428" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="9429" max="9429" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9430" max="9430" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9431" max="9431" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9432" max="9432" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9433" max="9433" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9434" max="9434" width="15.58203125" style="4" customWidth="1"/>
+    <col min="9435" max="9668" width="9" style="4"/>
+    <col min="9669" max="9669" width="37.83203125" style="4" customWidth="1"/>
+    <col min="9670" max="9670" width="6.58203125" style="4" customWidth="1"/>
+    <col min="9671" max="9671" width="9" style="4"/>
+    <col min="9672" max="9672" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9673" max="9673" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9674" max="9674" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9675" max="9675" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9676" max="9676" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9677" max="9677" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9678" max="9678" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="9679" max="9679" width="12.75" style="4" customWidth="1"/>
+    <col min="9680" max="9680" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9681" max="9681" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9682" max="9682" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9683" max="9683" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="9684" max="9684" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="9685" max="9685" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9686" max="9686" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9687" max="9687" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9688" max="9688" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9689" max="9689" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9690" max="9690" width="15.58203125" style="4" customWidth="1"/>
+    <col min="9691" max="9924" width="9" style="4"/>
+    <col min="9925" max="9925" width="37.83203125" style="4" customWidth="1"/>
+    <col min="9926" max="9926" width="6.58203125" style="4" customWidth="1"/>
+    <col min="9927" max="9927" width="9" style="4"/>
+    <col min="9928" max="9928" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9929" max="9929" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9930" max="9930" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9931" max="9931" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9932" max="9932" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9933" max="9933" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9934" max="9934" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="9935" max="9935" width="12.75" style="4" customWidth="1"/>
+    <col min="9936" max="9936" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9937" max="9937" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9938" max="9938" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9939" max="9939" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="9940" max="9940" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="9941" max="9941" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9942" max="9942" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9943" max="9943" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9944" max="9944" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9945" max="9945" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9946" max="9946" width="15.58203125" style="4" customWidth="1"/>
+    <col min="9947" max="10180" width="9" style="4"/>
+    <col min="10181" max="10181" width="37.83203125" style="4" customWidth="1"/>
+    <col min="10182" max="10182" width="6.58203125" style="4" customWidth="1"/>
+    <col min="10183" max="10183" width="9" style="4"/>
+    <col min="10184" max="10184" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10185" max="10185" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10186" max="10186" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10187" max="10187" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10188" max="10188" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10189" max="10189" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10190" max="10190" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="10191" max="10191" width="12.75" style="4" customWidth="1"/>
+    <col min="10192" max="10192" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10193" max="10193" width="14.08203125" style="4" customWidth="1"/>
+    <col min="10194" max="10194" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10195" max="10195" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="10196" max="10196" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="10197" max="10197" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10198" max="10198" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10199" max="10199" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10200" max="10200" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10201" max="10201" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10202" max="10202" width="15.58203125" style="4" customWidth="1"/>
+    <col min="10203" max="10436" width="9" style="4"/>
+    <col min="10437" max="10437" width="37.83203125" style="4" customWidth="1"/>
+    <col min="10438" max="10438" width="6.58203125" style="4" customWidth="1"/>
+    <col min="10439" max="10439" width="9" style="4"/>
+    <col min="10440" max="10440" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10441" max="10441" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10442" max="10442" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10443" max="10443" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10444" max="10444" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10445" max="10445" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10446" max="10446" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="10447" max="10447" width="12.75" style="4" customWidth="1"/>
+    <col min="10448" max="10448" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10449" max="10449" width="14.08203125" style="4" customWidth="1"/>
+    <col min="10450" max="10450" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10451" max="10451" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="10452" max="10452" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="10453" max="10453" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10454" max="10454" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10455" max="10455" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10456" max="10456" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10457" max="10457" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10458" max="10458" width="15.58203125" style="4" customWidth="1"/>
+    <col min="10459" max="10692" width="9" style="4"/>
+    <col min="10693" max="10693" width="37.83203125" style="4" customWidth="1"/>
+    <col min="10694" max="10694" width="6.58203125" style="4" customWidth="1"/>
+    <col min="10695" max="10695" width="9" style="4"/>
+    <col min="10696" max="10696" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10697" max="10697" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10698" max="10698" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10699" max="10699" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10700" max="10700" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10701" max="10701" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10702" max="10702" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="10703" max="10703" width="12.75" style="4" customWidth="1"/>
+    <col min="10704" max="10704" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10705" max="10705" width="14.08203125" style="4" customWidth="1"/>
+    <col min="10706" max="10706" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10707" max="10707" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="10708" max="10708" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="10709" max="10709" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10710" max="10710" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10711" max="10711" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10712" max="10712" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10713" max="10713" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10714" max="10714" width="15.58203125" style="4" customWidth="1"/>
+    <col min="10715" max="10948" width="9" style="4"/>
+    <col min="10949" max="10949" width="37.83203125" style="4" customWidth="1"/>
+    <col min="10950" max="10950" width="6.58203125" style="4" customWidth="1"/>
+    <col min="10951" max="10951" width="9" style="4"/>
+    <col min="10952" max="10952" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10953" max="10953" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10954" max="10954" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10955" max="10955" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10956" max="10956" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10957" max="10957" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10958" max="10958" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="10959" max="10959" width="12.75" style="4" customWidth="1"/>
+    <col min="10960" max="10960" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10961" max="10961" width="14.08203125" style="4" customWidth="1"/>
+    <col min="10962" max="10962" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10963" max="10963" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="10964" max="10964" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="10965" max="10965" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10966" max="10966" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10967" max="10967" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10968" max="10968" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10969" max="10969" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10970" max="10970" width="15.58203125" style="4" customWidth="1"/>
+    <col min="10971" max="11204" width="9" style="4"/>
+    <col min="11205" max="11205" width="37.83203125" style="4" customWidth="1"/>
+    <col min="11206" max="11206" width="6.58203125" style="4" customWidth="1"/>
+    <col min="11207" max="11207" width="9" style="4"/>
+    <col min="11208" max="11208" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11209" max="11209" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11210" max="11210" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11211" max="11211" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="11212" max="11212" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11213" max="11213" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11214" max="11214" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11215" max="11215" width="12.75" style="4" customWidth="1"/>
+    <col min="11216" max="11216" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11217" max="11217" width="14.08203125" style="4" customWidth="1"/>
+    <col min="11218" max="11218" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11219" max="11219" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="11220" max="11220" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="11221" max="11221" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11222" max="11222" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11223" max="11223" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11224" max="11224" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11225" max="11225" width="12.83203125" style="4" customWidth="1"/>
+    <col min="11226" max="11226" width="15.58203125" style="4" customWidth="1"/>
+    <col min="11227" max="11460" width="9" style="4"/>
+    <col min="11461" max="11461" width="37.83203125" style="4" customWidth="1"/>
+    <col min="11462" max="11462" width="6.58203125" style="4" customWidth="1"/>
+    <col min="11463" max="11463" width="9" style="4"/>
+    <col min="11464" max="11464" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11465" max="11465" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11466" max="11466" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11467" max="11467" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="11468" max="11468" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11469" max="11469" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11470" max="11470" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11471" max="11471" width="12.75" style="4" customWidth="1"/>
+    <col min="11472" max="11472" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11473" max="11473" width="14.08203125" style="4" customWidth="1"/>
+    <col min="11474" max="11474" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11475" max="11475" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="11476" max="11476" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="11477" max="11477" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11478" max="11478" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11479" max="11479" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11480" max="11480" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11481" max="11481" width="12.83203125" style="4" customWidth="1"/>
+    <col min="11482" max="11482" width="15.58203125" style="4" customWidth="1"/>
+    <col min="11483" max="11716" width="9" style="4"/>
+    <col min="11717" max="11717" width="37.83203125" style="4" customWidth="1"/>
+    <col min="11718" max="11718" width="6.58203125" style="4" customWidth="1"/>
+    <col min="11719" max="11719" width="9" style="4"/>
+    <col min="11720" max="11720" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11721" max="11721" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11722" max="11722" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11723" max="11723" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="11724" max="11724" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11725" max="11725" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11726" max="11726" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11727" max="11727" width="12.75" style="4" customWidth="1"/>
+    <col min="11728" max="11728" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11729" max="11729" width="14.08203125" style="4" customWidth="1"/>
+    <col min="11730" max="11730" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11731" max="11731" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="11732" max="11732" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="11733" max="11733" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11734" max="11734" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11735" max="11735" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11736" max="11736" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11737" max="11737" width="12.83203125" style="4" customWidth="1"/>
+    <col min="11738" max="11738" width="15.58203125" style="4" customWidth="1"/>
+    <col min="11739" max="11972" width="9" style="4"/>
+    <col min="11973" max="11973" width="37.83203125" style="4" customWidth="1"/>
+    <col min="11974" max="11974" width="6.58203125" style="4" customWidth="1"/>
+    <col min="11975" max="11975" width="9" style="4"/>
+    <col min="11976" max="11976" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11977" max="11977" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11978" max="11978" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11979" max="11979" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="11980" max="11980" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11981" max="11981" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11982" max="11982" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11983" max="11983" width="12.75" style="4" customWidth="1"/>
+    <col min="11984" max="11984" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11985" max="11985" width="14.08203125" style="4" customWidth="1"/>
+    <col min="11986" max="11986" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11987" max="11987" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="11988" max="11988" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="11989" max="11989" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11990" max="11990" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11991" max="11991" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11992" max="11992" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11993" max="11993" width="12.83203125" style="4" customWidth="1"/>
+    <col min="11994" max="11994" width="15.58203125" style="4" customWidth="1"/>
+    <col min="11995" max="12228" width="9" style="4"/>
+    <col min="12229" max="12229" width="37.83203125" style="4" customWidth="1"/>
+    <col min="12230" max="12230" width="6.58203125" style="4" customWidth="1"/>
+    <col min="12231" max="12231" width="9" style="4"/>
+    <col min="12232" max="12232" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12233" max="12233" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12234" max="12234" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12235" max="12235" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="12236" max="12236" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12237" max="12237" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12238" max="12238" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="12239" max="12239" width="12.75" style="4" customWidth="1"/>
+    <col min="12240" max="12240" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12241" max="12241" width="14.08203125" style="4" customWidth="1"/>
+    <col min="12242" max="12242" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12243" max="12243" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="12244" max="12244" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="12245" max="12245" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12246" max="12246" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12247" max="12247" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12248" max="12248" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12249" max="12249" width="12.83203125" style="4" customWidth="1"/>
+    <col min="12250" max="12250" width="15.58203125" style="4" customWidth="1"/>
+    <col min="12251" max="12484" width="9" style="4"/>
+    <col min="12485" max="12485" width="37.83203125" style="4" customWidth="1"/>
+    <col min="12486" max="12486" width="6.58203125" style="4" customWidth="1"/>
+    <col min="12487" max="12487" width="9" style="4"/>
+    <col min="12488" max="12488" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12489" max="12489" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12490" max="12490" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12491" max="12491" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="12492" max="12492" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12493" max="12493" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12494" max="12494" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="12495" max="12495" width="12.75" style="4" customWidth="1"/>
+    <col min="12496" max="12496" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12497" max="12497" width="14.08203125" style="4" customWidth="1"/>
+    <col min="12498" max="12498" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12499" max="12499" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="12500" max="12500" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="12501" max="12501" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12502" max="12502" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12503" max="12503" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12504" max="12504" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12505" max="12505" width="12.83203125" style="4" customWidth="1"/>
+    <col min="12506" max="12506" width="15.58203125" style="4" customWidth="1"/>
+    <col min="12507" max="12740" width="9" style="4"/>
+    <col min="12741" max="12741" width="37.83203125" style="4" customWidth="1"/>
+    <col min="12742" max="12742" width="6.58203125" style="4" customWidth="1"/>
+    <col min="12743" max="12743" width="9" style="4"/>
+    <col min="12744" max="12744" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12745" max="12745" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12746" max="12746" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12747" max="12747" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="12748" max="12748" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12749" max="12749" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12750" max="12750" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="12751" max="12751" width="12.75" style="4" customWidth="1"/>
+    <col min="12752" max="12752" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12753" max="12753" width="14.08203125" style="4" customWidth="1"/>
+    <col min="12754" max="12754" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12755" max="12755" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="12756" max="12756" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="12757" max="12757" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12758" max="12758" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12759" max="12759" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12760" max="12760" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12761" max="12761" width="12.83203125" style="4" customWidth="1"/>
+    <col min="12762" max="12762" width="15.58203125" style="4" customWidth="1"/>
+    <col min="12763" max="12996" width="9" style="4"/>
+    <col min="12997" max="12997" width="37.83203125" style="4" customWidth="1"/>
+    <col min="12998" max="12998" width="6.58203125" style="4" customWidth="1"/>
+    <col min="12999" max="12999" width="9" style="4"/>
+    <col min="13000" max="13000" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13001" max="13001" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13002" max="13002" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13003" max="13003" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="13004" max="13004" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13005" max="13005" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13006" max="13006" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="13007" max="13007" width="12.75" style="4" customWidth="1"/>
+    <col min="13008" max="13008" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13009" max="13009" width="14.08203125" style="4" customWidth="1"/>
+    <col min="13010" max="13010" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13011" max="13011" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13012" max="13012" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="13013" max="13013" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13014" max="13014" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13015" max="13015" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13016" max="13016" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13017" max="13017" width="12.83203125" style="4" customWidth="1"/>
+    <col min="13018" max="13018" width="15.58203125" style="4" customWidth="1"/>
+    <col min="13019" max="13252" width="9" style="4"/>
+    <col min="13253" max="13253" width="37.83203125" style="4" customWidth="1"/>
+    <col min="13254" max="13254" width="6.58203125" style="4" customWidth="1"/>
+    <col min="13255" max="13255" width="9" style="4"/>
+    <col min="13256" max="13256" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13257" max="13257" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13258" max="13258" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13259" max="13259" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="13260" max="13260" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13261" max="13261" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13262" max="13262" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="13263" max="13263" width="12.75" style="4" customWidth="1"/>
+    <col min="13264" max="13264" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13265" max="13265" width="14.08203125" style="4" customWidth="1"/>
+    <col min="13266" max="13266" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13267" max="13267" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13268" max="13268" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="13269" max="13269" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13270" max="13270" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13271" max="13271" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13272" max="13272" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13273" max="13273" width="12.83203125" style="4" customWidth="1"/>
+    <col min="13274" max="13274" width="15.58203125" style="4" customWidth="1"/>
+    <col min="13275" max="13508" width="9" style="4"/>
+    <col min="13509" max="13509" width="37.83203125" style="4" customWidth="1"/>
+    <col min="13510" max="13510" width="6.58203125" style="4" customWidth="1"/>
+    <col min="13511" max="13511" width="9" style="4"/>
+    <col min="13512" max="13512" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13513" max="13513" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13514" max="13514" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13515" max="13515" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="13516" max="13516" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13517" max="13517" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13518" max="13518" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="13519" max="13519" width="12.75" style="4" customWidth="1"/>
+    <col min="13520" max="13520" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13521" max="13521" width="14.08203125" style="4" customWidth="1"/>
+    <col min="13522" max="13522" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13523" max="13523" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13524" max="13524" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="13525" max="13525" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13526" max="13526" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13527" max="13527" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13528" max="13528" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13529" max="13529" width="12.83203125" style="4" customWidth="1"/>
+    <col min="13530" max="13530" width="15.58203125" style="4" customWidth="1"/>
+    <col min="13531" max="13764" width="9" style="4"/>
+    <col min="13765" max="13765" width="37.83203125" style="4" customWidth="1"/>
+    <col min="13766" max="13766" width="6.58203125" style="4" customWidth="1"/>
+    <col min="13767" max="13767" width="9" style="4"/>
+    <col min="13768" max="13768" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13769" max="13769" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13770" max="13770" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13771" max="13771" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="13772" max="13772" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13773" max="13773" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13774" max="13774" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="13775" max="13775" width="12.75" style="4" customWidth="1"/>
+    <col min="13776" max="13776" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13777" max="13777" width="14.08203125" style="4" customWidth="1"/>
+    <col min="13778" max="13778" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13779" max="13779" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13780" max="13780" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="13781" max="13781" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13782" max="13782" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13783" max="13783" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13784" max="13784" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13785" max="13785" width="12.83203125" style="4" customWidth="1"/>
+    <col min="13786" max="13786" width="15.58203125" style="4" customWidth="1"/>
+    <col min="13787" max="14020" width="9" style="4"/>
+    <col min="14021" max="14021" width="37.83203125" style="4" customWidth="1"/>
+    <col min="14022" max="14022" width="6.58203125" style="4" customWidth="1"/>
+    <col min="14023" max="14023" width="9" style="4"/>
+    <col min="14024" max="14024" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14025" max="14025" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14026" max="14026" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14027" max="14027" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="14028" max="14028" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14029" max="14029" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14030" max="14030" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="14031" max="14031" width="12.75" style="4" customWidth="1"/>
+    <col min="14032" max="14032" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14033" max="14033" width="14.08203125" style="4" customWidth="1"/>
+    <col min="14034" max="14034" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14035" max="14035" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="14036" max="14036" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="14037" max="14037" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14038" max="14038" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14039" max="14039" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14040" max="14040" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14041" max="14041" width="12.83203125" style="4" customWidth="1"/>
+    <col min="14042" max="14042" width="15.58203125" style="4" customWidth="1"/>
+    <col min="14043" max="14276" width="9" style="4"/>
+    <col min="14277" max="14277" width="37.83203125" style="4" customWidth="1"/>
+    <col min="14278" max="14278" width="6.58203125" style="4" customWidth="1"/>
+    <col min="14279" max="14279" width="9" style="4"/>
+    <col min="14280" max="14280" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14281" max="14281" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14282" max="14282" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14283" max="14283" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="14284" max="14284" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14285" max="14285" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14286" max="14286" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="14287" max="14287" width="12.75" style="4" customWidth="1"/>
+    <col min="14288" max="14288" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14289" max="14289" width="14.08203125" style="4" customWidth="1"/>
+    <col min="14290" max="14290" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14291" max="14291" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="14292" max="14292" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="14293" max="14293" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14294" max="14294" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14295" max="14295" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14296" max="14296" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14297" max="14297" width="12.83203125" style="4" customWidth="1"/>
+    <col min="14298" max="14298" width="15.58203125" style="4" customWidth="1"/>
+    <col min="14299" max="14532" width="9" style="4"/>
+    <col min="14533" max="14533" width="37.83203125" style="4" customWidth="1"/>
+    <col min="14534" max="14534" width="6.58203125" style="4" customWidth="1"/>
+    <col min="14535" max="14535" width="9" style="4"/>
+    <col min="14536" max="14536" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14537" max="14537" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14538" max="14538" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14539" max="14539" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="14540" max="14540" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14541" max="14541" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14542" max="14542" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="14543" max="14543" width="12.75" style="4" customWidth="1"/>
+    <col min="14544" max="14544" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14545" max="14545" width="14.08203125" style="4" customWidth="1"/>
+    <col min="14546" max="14546" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14547" max="14547" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="14548" max="14548" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="14549" max="14549" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14550" max="14550" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14551" max="14551" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14552" max="14552" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14553" max="14553" width="12.83203125" style="4" customWidth="1"/>
+    <col min="14554" max="14554" width="15.58203125" style="4" customWidth="1"/>
+    <col min="14555" max="14788" width="9" style="4"/>
+    <col min="14789" max="14789" width="37.83203125" style="4" customWidth="1"/>
+    <col min="14790" max="14790" width="6.58203125" style="4" customWidth="1"/>
+    <col min="14791" max="14791" width="9" style="4"/>
+    <col min="14792" max="14792" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14793" max="14793" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14794" max="14794" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14795" max="14795" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="14796" max="14796" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14797" max="14797" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14798" max="14798" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="14799" max="14799" width="12.75" style="4" customWidth="1"/>
+    <col min="14800" max="14800" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14801" max="14801" width="14.08203125" style="4" customWidth="1"/>
+    <col min="14802" max="14802" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14803" max="14803" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="14804" max="14804" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="14805" max="14805" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14806" max="14806" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14807" max="14807" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14808" max="14808" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14809" max="14809" width="12.83203125" style="4" customWidth="1"/>
+    <col min="14810" max="14810" width="15.58203125" style="4" customWidth="1"/>
+    <col min="14811" max="15044" width="9" style="4"/>
+    <col min="15045" max="15045" width="37.83203125" style="4" customWidth="1"/>
+    <col min="15046" max="15046" width="6.58203125" style="4" customWidth="1"/>
+    <col min="15047" max="15047" width="9" style="4"/>
+    <col min="15048" max="15048" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15049" max="15049" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15050" max="15050" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15051" max="15051" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="15052" max="15052" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15053" max="15053" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15054" max="15054" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="15055" max="15055" width="12.75" style="4" customWidth="1"/>
+    <col min="15056" max="15056" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15057" max="15057" width="14.08203125" style="4" customWidth="1"/>
+    <col min="15058" max="15058" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15059" max="15059" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="15060" max="15060" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15061" max="15061" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15062" max="15062" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15063" max="15063" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15064" max="15064" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15065" max="15065" width="12.83203125" style="4" customWidth="1"/>
+    <col min="15066" max="15066" width="15.58203125" style="4" customWidth="1"/>
+    <col min="15067" max="15300" width="9" style="4"/>
+    <col min="15301" max="15301" width="37.83203125" style="4" customWidth="1"/>
+    <col min="15302" max="15302" width="6.58203125" style="4" customWidth="1"/>
+    <col min="15303" max="15303" width="9" style="4"/>
+    <col min="15304" max="15304" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15305" max="15305" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15306" max="15306" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15307" max="15307" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="15308" max="15308" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15309" max="15309" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15310" max="15310" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="15311" max="15311" width="12.75" style="4" customWidth="1"/>
+    <col min="15312" max="15312" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15313" max="15313" width="14.08203125" style="4" customWidth="1"/>
+    <col min="15314" max="15314" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15315" max="15315" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="15316" max="15316" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15317" max="15317" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15318" max="15318" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15319" max="15319" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15320" max="15320" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15321" max="15321" width="12.83203125" style="4" customWidth="1"/>
+    <col min="15322" max="15322" width="15.58203125" style="4" customWidth="1"/>
+    <col min="15323" max="15556" width="9" style="4"/>
+    <col min="15557" max="15557" width="37.83203125" style="4" customWidth="1"/>
+    <col min="15558" max="15558" width="6.58203125" style="4" customWidth="1"/>
+    <col min="15559" max="15559" width="9" style="4"/>
+    <col min="15560" max="15560" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15561" max="15561" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15562" max="15562" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15563" max="15563" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="15564" max="15564" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15565" max="15565" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15566" max="15566" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="15567" max="15567" width="12.75" style="4" customWidth="1"/>
+    <col min="15568" max="15568" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15569" max="15569" width="14.08203125" style="4" customWidth="1"/>
+    <col min="15570" max="15570" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15571" max="15571" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="15572" max="15572" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15573" max="15573" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15574" max="15574" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15575" max="15575" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15576" max="15576" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15577" max="15577" width="12.83203125" style="4" customWidth="1"/>
+    <col min="15578" max="15578" width="15.58203125" style="4" customWidth="1"/>
+    <col min="15579" max="15812" width="9" style="4"/>
+    <col min="15813" max="15813" width="37.83203125" style="4" customWidth="1"/>
+    <col min="15814" max="15814" width="6.58203125" style="4" customWidth="1"/>
+    <col min="15815" max="15815" width="9" style="4"/>
+    <col min="15816" max="15816" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15817" max="15817" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15818" max="15818" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15819" max="15819" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="15820" max="15820" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15821" max="15821" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15822" max="15822" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="15823" max="15823" width="12.75" style="4" customWidth="1"/>
+    <col min="15824" max="15824" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15825" max="15825" width="14.08203125" style="4" customWidth="1"/>
+    <col min="15826" max="15826" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15827" max="15827" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="15828" max="15828" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15829" max="15829" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15830" max="15830" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15831" max="15831" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15832" max="15832" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15833" max="15833" width="12.83203125" style="4" customWidth="1"/>
+    <col min="15834" max="15834" width="15.58203125" style="4" customWidth="1"/>
+    <col min="15835" max="16068" width="9" style="4"/>
+    <col min="16069" max="16069" width="37.83203125" style="4" customWidth="1"/>
+    <col min="16070" max="16070" width="6.58203125" style="4" customWidth="1"/>
+    <col min="16071" max="16071" width="9" style="4"/>
+    <col min="16072" max="16072" width="7.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16073" max="16073" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16074" max="16074" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16075" max="16075" width="11.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="16076" max="16076" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16077" max="16077" width="13.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16078" max="16078" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="16079" max="16079" width="12.75" style="4" customWidth="1"/>
+    <col min="16080" max="16080" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16081" max="16081" width="14.08203125" style="4" customWidth="1"/>
+    <col min="16082" max="16082" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16083" max="16083" width="13.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="16084" max="16084" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="16085" max="16085" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16086" max="16086" width="10.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16087" max="16087" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16088" max="16088" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16089" max="16089" width="12.83203125" style="4" customWidth="1"/>
+    <col min="16090" max="16090" width="15.58203125" style="4" customWidth="1"/>
+    <col min="16091" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -3968,7 +3968,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:21">

</xml_diff>